<commit_message>
employment and earnings update
</commit_message>
<xml_diff>
--- a/data/historical/source/earnings_historical.xlsx
+++ b/data/historical/source/earnings_historical.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EHuffer\Box Sync\TPC\CENTER\SLFI\Interactive Data Tools\SEM\Historical\Earnings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\aboddupalli\Box Sync\TPC\CENTER\SLFI\Interactive Data Tools\SEM\Historical\Earnings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -183,7 +183,7 @@
     <t>Wyoming</t>
   </si>
   <si>
-    <t>Real Average Weekly Wages; Year/Year: January 2008 -- September 2018</t>
+    <t>Real Average Weekly Wages; Year/Year: January 2008 -- October 2018</t>
   </si>
 </sst>
 </file>
@@ -2422,11 +2422,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA134"/>
+  <dimension ref="A1:BA135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B134" sqref="B134:BA134"/>
+      <pane ySplit="5" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20015,160 +20015,160 @@
         <v>42736</v>
       </c>
       <c r="B114" s="6">
-        <v>-0.67149127751743742</v>
+        <v>-0.67149127751745397</v>
       </c>
       <c r="C114" s="6">
-        <v>1.0177689751490016</v>
+        <v>1.0177689751489818</v>
       </c>
       <c r="D114" s="6">
-        <v>1.8156403017748333</v>
+        <v>1.8156403017748199</v>
       </c>
       <c r="E114" s="6">
-        <v>4.1673704069850928</v>
+        <v>4.1673704069850732</v>
       </c>
       <c r="F114" s="6">
-        <v>1.5711398732707726</v>
+        <v>1.5711398732707629</v>
       </c>
       <c r="G114" s="6">
-        <v>3.2682622110002009</v>
+        <v>3.2682622110001862</v>
       </c>
       <c r="H114" s="6">
-        <v>-3.2798774422086625</v>
+        <v>-3.2798774422086696</v>
       </c>
       <c r="I114" s="6">
-        <v>2.5617461407898232</v>
+        <v>2.5617461407897979</v>
       </c>
       <c r="J114" s="6">
-        <v>1.6894524971481355</v>
+        <v>1.6894524971481089</v>
       </c>
       <c r="K114" s="6">
-        <v>12.176204136486959</v>
+        <v>12.176204136486952</v>
       </c>
       <c r="L114" s="6">
-        <v>3.18213807697899</v>
+        <v>3.1821380769789833</v>
       </c>
       <c r="M114" s="6">
-        <v>2.969235003035029</v>
+        <v>2.969235003035013</v>
       </c>
       <c r="N114" s="6">
-        <v>2.7904353632908547</v>
+        <v>2.7904353632908339</v>
       </c>
       <c r="O114" s="6">
-        <v>-1.966202849758645</v>
+        <v>-1.9662028497586588</v>
       </c>
       <c r="P114" s="6">
-        <v>-1.0055240871695621</v>
+        <v>-1.0055240871695768</v>
       </c>
       <c r="Q114" s="6">
-        <v>2.6285162780659372</v>
+        <v>2.6285162780659301</v>
       </c>
       <c r="R114" s="6">
-        <v>0.93582441639476122</v>
+        <v>0.93582441639475344</v>
       </c>
       <c r="S114" s="6">
-        <v>-0.44521435734071435</v>
+        <v>-0.44521435734074094</v>
       </c>
       <c r="T114" s="6">
-        <v>2.0834355923945536</v>
+        <v>2.0834355923945402</v>
       </c>
       <c r="U114" s="6">
-        <v>0.35909012695466452</v>
+        <v>0.35909012695464254</v>
       </c>
       <c r="V114" s="6">
-        <v>0.87175029420872752</v>
+        <v>0.87175029420871031</v>
       </c>
       <c r="W114" s="6">
-        <v>2.9842277572997897</v>
+        <v>2.98422775729978</v>
       </c>
       <c r="X114" s="6">
-        <v>1.5705713441556988</v>
+        <v>1.5705713441556732</v>
       </c>
       <c r="Y114" s="6">
-        <v>0.96599034519679239</v>
+        <v>0.96599034519677329</v>
       </c>
       <c r="Z114" s="6">
-        <v>4.5400875006239589</v>
+        <v>4.5400875006239394</v>
       </c>
       <c r="AA114" s="6">
-        <v>1.0319761338320388</v>
+        <v>1.031976133832035</v>
       </c>
       <c r="AB114" s="6">
-        <v>4.0278017193327917</v>
+        <v>4.0278017193327669</v>
       </c>
       <c r="AC114" s="6">
-        <v>2.6940671461368639</v>
+        <v>2.6940671461368493</v>
       </c>
       <c r="AD114" s="6">
-        <v>3.6775843635426719</v>
+        <v>3.6775843635426511</v>
       </c>
       <c r="AE114" s="6">
-        <v>2.0940831307987233</v>
+        <v>2.0940831307987082</v>
       </c>
       <c r="AF114" s="6">
-        <v>2.466151647608446</v>
+        <v>2.4661516476084357</v>
       </c>
       <c r="AG114" s="6">
-        <v>4.7667198501047894</v>
+        <v>4.7667198501047583</v>
       </c>
       <c r="AH114" s="6">
-        <v>-0.24585512855784605</v>
+        <v>-0.24585512855786812</v>
       </c>
       <c r="AI114" s="6">
-        <v>0.86439594349482418</v>
+        <v>0.86439594349481186</v>
       </c>
       <c r="AJ114" s="6">
-        <v>2.7946619906369996</v>
+        <v>2.7946619906369832</v>
       </c>
       <c r="AK114" s="6">
-        <v>-4.2406825010564591</v>
+        <v>-4.2406825010564768</v>
       </c>
       <c r="AL114" s="6">
-        <v>2.5079877529563266</v>
+        <v>2.5079877529563146</v>
       </c>
       <c r="AM114" s="6">
-        <v>2.9144801806287304</v>
+        <v>2.9144801806287224</v>
       </c>
       <c r="AN114" s="6">
-        <v>4.7821931511225619</v>
+        <v>4.7821931511225415</v>
       </c>
       <c r="AO114" s="6">
-        <v>-0.42184923653606349</v>
+        <v>-0.42184923653607997</v>
       </c>
       <c r="AP114" s="6">
-        <v>1.5244063651617707</v>
+        <v>1.5244063651617519</v>
       </c>
       <c r="AQ114" s="6">
-        <v>2.958149599632371</v>
+        <v>2.9581495996323648</v>
       </c>
       <c r="AR114" s="6">
-        <v>1.4741491567979961</v>
+        <v>1.4741491567979965</v>
       </c>
       <c r="AS114" s="6">
-        <v>5.4707214644460525</v>
+        <v>5.4707214644460418</v>
       </c>
       <c r="AT114" s="6">
-        <v>1.182418713104235</v>
+        <v>1.1824187131042243</v>
       </c>
       <c r="AU114" s="6">
-        <v>2.1590798473481008</v>
+        <v>2.1590798473480906</v>
       </c>
       <c r="AV114" s="6">
-        <v>-2.137906128845307</v>
+        <v>-2.1379061288453216</v>
       </c>
       <c r="AW114" s="6">
-        <v>2.4315417351543882</v>
+        <v>2.4315417351543722</v>
       </c>
       <c r="AX114" s="6">
-        <v>3.5047064947352204</v>
+        <v>3.5047064947351951</v>
       </c>
       <c r="AY114" s="6">
-        <v>2.1755051606674392</v>
+        <v>2.175505160667432</v>
       </c>
       <c r="AZ114" s="6">
-        <v>1.9255747589039096</v>
+        <v>1.9255747589038938</v>
       </c>
       <c r="BA114" s="6">
-        <v>0.35810966669563454</v>
+        <v>0.35810966669562688</v>
       </c>
     </row>
     <row r="115" spans="1:53" x14ac:dyDescent="0.2">
@@ -20176,160 +20176,160 @@
         <v>42767</v>
       </c>
       <c r="B115" s="6">
-        <v>-0.30834653044826943</v>
+        <v>-0.30834653044827015</v>
       </c>
       <c r="C115" s="6">
-        <v>-0.55110469438561693</v>
+        <v>-0.55110469438563225</v>
       </c>
       <c r="D115" s="6">
-        <v>-1.0051164683987055</v>
+        <v>-1.0051164683987068</v>
       </c>
       <c r="E115" s="6">
-        <v>2.7977484892839128</v>
+        <v>2.797748489283908</v>
       </c>
       <c r="F115" s="6">
-        <v>1.6519897674419144</v>
+        <v>1.6519897674418988</v>
       </c>
       <c r="G115" s="6">
-        <v>0.17872856411678109</v>
+        <v>0.17872856411679391</v>
       </c>
       <c r="H115" s="6">
-        <v>-3.6490145906076341</v>
+        <v>-3.6490145906076319</v>
       </c>
       <c r="I115" s="6">
-        <v>0.17769204455070722</v>
+        <v>0.17769204455072055</v>
       </c>
       <c r="J115" s="6">
-        <v>0.7782802737514074</v>
+        <v>0.77828027375139974</v>
       </c>
       <c r="K115" s="6">
-        <v>5.6466326079205356</v>
+        <v>5.646632607920548</v>
       </c>
       <c r="L115" s="6">
-        <v>1.7147725836171968</v>
+        <v>1.7147725836171974</v>
       </c>
       <c r="M115" s="6">
-        <v>0.19090195490322329</v>
+        <v>0.19090195490321982</v>
       </c>
       <c r="N115" s="6">
-        <v>-1.202221780160563</v>
+        <v>-1.2022217801605628</v>
       </c>
       <c r="O115" s="6">
-        <v>-1.931294085450765</v>
+        <v>-1.9312940854507601</v>
       </c>
       <c r="P115" s="6">
-        <v>-2.1826771984394084</v>
+        <v>-2.1826771984394235</v>
       </c>
       <c r="Q115" s="6">
-        <v>2.6637497466305065</v>
+        <v>2.663749746630502</v>
       </c>
       <c r="R115" s="6">
-        <v>-6.9560071884794294E-2</v>
+        <v>-6.9560071884804189E-2</v>
       </c>
       <c r="S115" s="6">
-        <v>-0.12107352301745707</v>
+        <v>-0.12107352301746362</v>
       </c>
       <c r="T115" s="6">
-        <v>0.76681461564566855</v>
+        <v>0.76681461564564679</v>
       </c>
       <c r="U115" s="6">
-        <v>0.97257730295085465</v>
+        <v>0.9725773029508481</v>
       </c>
       <c r="V115" s="6">
-        <v>0.48662774331923148</v>
+        <v>0.48662774331922248</v>
       </c>
       <c r="W115" s="6">
-        <v>1.2171951979874058</v>
+        <v>1.2171951979874045</v>
       </c>
       <c r="X115" s="6">
-        <v>0.51202285686138727</v>
+        <v>0.51202285686137294</v>
       </c>
       <c r="Y115" s="6">
-        <v>0.45252494262051884</v>
+        <v>0.4525249426205174</v>
       </c>
       <c r="Z115" s="6">
-        <v>4.8840603679666801</v>
+        <v>4.8840603679666756</v>
       </c>
       <c r="AA115" s="6">
-        <v>1.0804809693970356</v>
+        <v>1.0804809693970343</v>
       </c>
       <c r="AB115" s="6">
-        <v>2.5111960116249854</v>
+        <v>2.5111960116249943</v>
       </c>
       <c r="AC115" s="6">
-        <v>-1.7978407974824591</v>
+        <v>-1.7978407974824746</v>
       </c>
       <c r="AD115" s="6">
-        <v>1.1739857405401601</v>
+        <v>1.1739857405401495</v>
       </c>
       <c r="AE115" s="6">
-        <v>-0.98028178282786105</v>
+        <v>-0.98028178282787359</v>
       </c>
       <c r="AF115" s="6">
-        <v>1.3306181013694649</v>
+        <v>1.3306181013694705</v>
       </c>
       <c r="AG115" s="6">
-        <v>-0.26592593860225761</v>
+        <v>-0.26592593860226293</v>
       </c>
       <c r="AH115" s="6">
-        <v>-2.1359513195486923</v>
+        <v>-2.1359513195486972</v>
       </c>
       <c r="AI115" s="6">
-        <v>-1.4113588186572747</v>
+        <v>-1.4113588186572827</v>
       </c>
       <c r="AJ115" s="6">
-        <v>2.4820309460933854</v>
+        <v>2.4820309460933774</v>
       </c>
       <c r="AK115" s="6">
-        <v>-3.7253853037233915</v>
+        <v>-3.7253853037233933</v>
       </c>
       <c r="AL115" s="6">
-        <v>0.91783870490956998</v>
+        <v>0.91783870490955555</v>
       </c>
       <c r="AM115" s="6">
-        <v>2.2166212529784146</v>
+        <v>2.2166212529784111</v>
       </c>
       <c r="AN115" s="6">
-        <v>3.0806915879238108</v>
+        <v>3.0806915879237957</v>
       </c>
       <c r="AO115" s="6">
-        <v>-1.177053098856832</v>
+        <v>-1.1770530988568344</v>
       </c>
       <c r="AP115" s="6">
-        <v>-1.2580499134378351</v>
+        <v>-1.2580499134378418</v>
       </c>
       <c r="AQ115" s="6">
-        <v>1.578595355213261</v>
+        <v>1.5785953552132526</v>
       </c>
       <c r="AR115" s="6">
-        <v>1.4573090410535072</v>
+        <v>1.4573090410535057</v>
       </c>
       <c r="AS115" s="6">
-        <v>4.1045677830122678</v>
+        <v>4.1045677830122553</v>
       </c>
       <c r="AT115" s="6">
-        <v>-0.55816378473205119</v>
+        <v>-0.55816378473205319</v>
       </c>
       <c r="AU115" s="6">
-        <v>-0.26275991027767215</v>
+        <v>-0.26275991027768247</v>
       </c>
       <c r="AV115" s="6">
-        <v>-3.2627565101996465</v>
+        <v>-3.2627565101996727</v>
       </c>
       <c r="AW115" s="6">
-        <v>0.77205915726764207</v>
+        <v>0.77205915726762353</v>
       </c>
       <c r="AX115" s="6">
-        <v>-3.3834053564679126E-2</v>
+        <v>-3.3834053564675295E-2</v>
       </c>
       <c r="AY115" s="6">
-        <v>1.2105565289480815</v>
+        <v>1.2105565289480802</v>
       </c>
       <c r="AZ115" s="6">
-        <v>-6.9949136771024004E-2</v>
+        <v>-6.9949136771036258E-2</v>
       </c>
       <c r="BA115" s="6">
-        <v>-1.7141303565858739</v>
+        <v>-1.7141303565858721</v>
       </c>
     </row>
     <row r="116" spans="1:53" x14ac:dyDescent="0.2">
@@ -20337,160 +20337,160 @@
         <v>42795</v>
       </c>
       <c r="B116" s="6">
-        <v>-0.12266273679049772</v>
+        <v>-0.12266273679049783</v>
       </c>
       <c r="C116" s="6">
-        <v>0.50957910970788578</v>
+        <v>0.50957910970789377</v>
       </c>
       <c r="D116" s="6">
-        <v>0.10172376901148152</v>
+        <v>0.10172376901148236</v>
       </c>
       <c r="E116" s="6">
-        <v>1.9654205462321221</v>
+        <v>1.9654205462321297</v>
       </c>
       <c r="F116" s="6">
-        <v>3.1662838178140582</v>
+        <v>3.1662838178140493</v>
       </c>
       <c r="G116" s="6">
-        <v>1.678391879801441</v>
+        <v>1.6783918798014177</v>
       </c>
       <c r="H116" s="6">
-        <v>-3.6753170231478283</v>
+        <v>-3.6753170231478292</v>
       </c>
       <c r="I116" s="6">
-        <v>0.94027664965883173</v>
+        <v>0.94027664965884339</v>
       </c>
       <c r="J116" s="6">
-        <v>0.25108315358038119</v>
+        <v>0.25108315358038341</v>
       </c>
       <c r="K116" s="6">
-        <v>5.6358578852652856</v>
+        <v>5.6358578852652892</v>
       </c>
       <c r="L116" s="6">
-        <v>0.75680291798605781</v>
+        <v>0.75680291798604749</v>
       </c>
       <c r="M116" s="6">
-        <v>0.3884790455598508</v>
+        <v>0.38847904555987056</v>
       </c>
       <c r="N116" s="6">
-        <v>-1.3031390268204854</v>
+        <v>-1.3031390268204774</v>
       </c>
       <c r="O116" s="6">
-        <v>-1.3396201128926164</v>
+        <v>-1.3396201128926148</v>
       </c>
       <c r="P116" s="6">
-        <v>-2.3873018109886162</v>
+        <v>-2.3873018109886188</v>
       </c>
       <c r="Q116" s="6">
-        <v>2.4847681565760902</v>
+        <v>2.4847681565760822</v>
       </c>
       <c r="R116" s="6">
-        <v>-1.2999737543346581</v>
+        <v>-1.2999737543346659</v>
       </c>
       <c r="S116" s="6">
-        <v>0.29124848010289256</v>
+        <v>0.29124848010290288</v>
       </c>
       <c r="T116" s="6">
         <v>-0.27209357333880257</v>
       </c>
       <c r="U116" s="6">
-        <v>2.5635817975592801</v>
+        <v>2.5635817975592756</v>
       </c>
       <c r="V116" s="6">
-        <v>2.4268667891596762</v>
+        <v>2.4268667891596727</v>
       </c>
       <c r="W116" s="6">
-        <v>8.2669142548550761E-2</v>
+        <v>8.266914254854725E-2</v>
       </c>
       <c r="X116" s="6">
-        <v>0.5579832774368767</v>
+        <v>0.55798327743689091</v>
       </c>
       <c r="Y116" s="6">
-        <v>0.17888798024809774</v>
+        <v>0.17888798024809438</v>
       </c>
       <c r="Z116" s="6">
-        <v>3.0296185888538036</v>
+        <v>3.0296185888537974</v>
       </c>
       <c r="AA116" s="6">
-        <v>1.6827238844548547</v>
+        <v>1.6827238844548418</v>
       </c>
       <c r="AB116" s="6">
-        <v>3.6479387655206938</v>
+        <v>3.6479387655206987</v>
       </c>
       <c r="AC116" s="6">
-        <v>0.33828686957778326</v>
+        <v>0.33828686957778475</v>
       </c>
       <c r="AD116" s="6">
-        <v>2.9985452102034342</v>
+        <v>2.9985452102034387</v>
       </c>
       <c r="AE116" s="6">
-        <v>0.64359214444735946</v>
+        <v>0.64359214444735768</v>
       </c>
       <c r="AF116" s="6">
-        <v>2.7841664002205886</v>
+        <v>2.7841664002205899</v>
       </c>
       <c r="AG116" s="6">
-        <v>-0.90024562772280325</v>
+        <v>-0.90024562772279926</v>
       </c>
       <c r="AH116" s="6">
-        <v>-0.57364836744654368</v>
+        <v>-0.57364836744652958</v>
       </c>
       <c r="AI116" s="6">
-        <v>-1.0609469945340633</v>
+        <v>-1.0609469945340422</v>
       </c>
       <c r="AJ116" s="6">
-        <v>1.7211585889051588</v>
+        <v>1.7211585889051597</v>
       </c>
       <c r="AK116" s="6">
-        <v>-2.2642626007259383</v>
+        <v>-2.2642626007259432</v>
       </c>
       <c r="AL116" s="6">
-        <v>1.1869282613310703</v>
+        <v>1.1869282613310712</v>
       </c>
       <c r="AM116" s="6">
-        <v>3.4120919772471718</v>
+        <v>3.4120919772471634</v>
       </c>
       <c r="AN116" s="6">
-        <v>3.4073626456487531</v>
+        <v>3.4073626456487442</v>
       </c>
       <c r="AO116" s="6">
-        <v>-1.4987629516958045</v>
+        <v>-1.4987629516958101</v>
       </c>
       <c r="AP116" s="6">
-        <v>0.48218172638161833</v>
+        <v>0.48218172638161061</v>
       </c>
       <c r="AQ116" s="6">
-        <v>1.566045193671874</v>
+        <v>1.5660451936718778</v>
       </c>
       <c r="AR116" s="6">
-        <v>0.73269735877600684</v>
+        <v>0.7326973587760115</v>
       </c>
       <c r="AS116" s="6">
-        <v>2.4346524075927771</v>
+        <v>2.4346524075927793</v>
       </c>
       <c r="AT116" s="6">
-        <v>0.95905969436995231</v>
+        <v>0.95905969436995642</v>
       </c>
       <c r="AU116" s="6">
-        <v>0.53186232697560543</v>
+        <v>0.53186232697559743</v>
       </c>
       <c r="AV116" s="6">
-        <v>-3.534284274921458</v>
+        <v>-3.5342842749214585</v>
       </c>
       <c r="AW116" s="6">
-        <v>-0.99071604187869788</v>
+        <v>-0.99071604187869966</v>
       </c>
       <c r="AX116" s="6">
-        <v>0.71110184679658439</v>
+        <v>0.71110184679659172</v>
       </c>
       <c r="AY116" s="6">
-        <v>1.2408464213136283</v>
+        <v>1.2408464213136343</v>
       </c>
       <c r="AZ116" s="6">
-        <v>0.29443327691079035</v>
+        <v>0.29443327691078314</v>
       </c>
       <c r="BA116" s="6">
-        <v>-1.5386165443660675</v>
+        <v>-1.5386165443660693</v>
       </c>
     </row>
     <row r="117" spans="1:53" x14ac:dyDescent="0.2">
@@ -20498,160 +20498,160 @@
         <v>42826</v>
       </c>
       <c r="B117" s="6">
-        <v>0.30100480064995788</v>
+        <v>0.30100480064996021</v>
       </c>
       <c r="C117" s="6">
-        <v>1.1089489306088181</v>
+        <v>1.1089489306088096</v>
       </c>
       <c r="D117" s="6">
-        <v>0.36826589816464866</v>
+        <v>0.36826589816464561</v>
       </c>
       <c r="E117" s="6">
-        <v>5.4373300553895643</v>
+        <v>5.4373300553895598</v>
       </c>
       <c r="F117" s="6">
-        <v>3.8629625777355416</v>
+        <v>3.8629625777355474</v>
       </c>
       <c r="G117" s="6">
-        <v>4.1391808727476072</v>
+        <v>4.1391808727476231</v>
       </c>
       <c r="H117" s="6">
-        <v>0.44448627002505547</v>
+        <v>0.4444862700250572</v>
       </c>
       <c r="I117" s="6">
-        <v>2.3168731004677423</v>
+        <v>2.3168731004677432</v>
       </c>
       <c r="J117" s="6">
-        <v>3.8652242690642256</v>
+        <v>3.8652242690642211</v>
       </c>
       <c r="K117" s="6">
-        <v>6.7539749111793581</v>
+        <v>6.7539749111793457</v>
       </c>
       <c r="L117" s="6">
-        <v>3.5424592787875042</v>
+        <v>3.5424592787874918</v>
       </c>
       <c r="M117" s="6">
-        <v>3.3839664334704964</v>
+        <v>3.3839664334705075</v>
       </c>
       <c r="N117" s="6">
-        <v>3.4162592019192402</v>
+        <v>3.4162592019192384</v>
       </c>
       <c r="O117" s="6">
-        <v>0.50503808760054891</v>
+        <v>0.50503808760054214</v>
       </c>
       <c r="P117" s="6">
-        <v>-9.0973723556403457E-2</v>
+        <v>-9.0973723556399627E-2</v>
       </c>
       <c r="Q117" s="6">
-        <v>3.0313323962502881</v>
+        <v>3.031332396250304</v>
       </c>
       <c r="R117" s="6">
-        <v>-1.4496796997801895</v>
+        <v>-1.4496796997802044</v>
       </c>
       <c r="S117" s="6">
-        <v>1.2881940411671136</v>
+        <v>1.2881940411671085</v>
       </c>
       <c r="T117" s="6">
-        <v>0.67464466745903628</v>
+        <v>0.6746446674590264</v>
       </c>
       <c r="U117" s="6">
-        <v>0.37155498318990693</v>
+        <v>0.37155498318991032</v>
       </c>
       <c r="V117" s="6">
-        <v>2.6681846110162097</v>
+        <v>2.6681846110162093</v>
       </c>
       <c r="W117" s="6">
-        <v>2.1302866588015363</v>
+        <v>2.1302866588015514</v>
       </c>
       <c r="X117" s="6">
-        <v>2.6383397995324258</v>
+        <v>2.6383397995324347</v>
       </c>
       <c r="Y117" s="6">
-        <v>2.2052766538982436</v>
+        <v>2.2052766538982422</v>
       </c>
       <c r="Z117" s="6">
-        <v>6.6088589224458634</v>
+        <v>6.6088589224458563</v>
       </c>
       <c r="AA117" s="6">
-        <v>0.82330819655069276</v>
+        <v>0.8233081965506921</v>
       </c>
       <c r="AB117" s="6">
-        <v>6.5149140787769362</v>
+        <v>6.5149140787769486</v>
       </c>
       <c r="AC117" s="6">
-        <v>2.7333552190622532</v>
+        <v>2.733355219062251</v>
       </c>
       <c r="AD117" s="6">
-        <v>4.4394467307528105</v>
+        <v>4.4394467307528069</v>
       </c>
       <c r="AE117" s="6">
-        <v>1.0546791304277434</v>
+        <v>1.0546791304277476</v>
       </c>
       <c r="AF117" s="6">
-        <v>4.2050302971755524</v>
+        <v>4.2050302971755489</v>
       </c>
       <c r="AG117" s="6">
-        <v>1.8666724128780208</v>
+        <v>1.8666724128780132</v>
       </c>
       <c r="AH117" s="6">
-        <v>2.8870069898720101</v>
+        <v>2.8870069898720128</v>
       </c>
       <c r="AI117" s="6">
-        <v>2.4596251590708054</v>
+        <v>2.4596251590708085</v>
       </c>
       <c r="AJ117" s="6">
-        <v>3.631631934645613</v>
+        <v>3.6316319346456063</v>
       </c>
       <c r="AK117" s="6">
-        <v>0.75510421822793161</v>
+        <v>0.75510421822792373</v>
       </c>
       <c r="AL117" s="6">
-        <v>0.73437736364029893</v>
+        <v>0.73437736364029182</v>
       </c>
       <c r="AM117" s="6">
-        <v>5.9595316908722982</v>
+        <v>5.9595316908723079</v>
       </c>
       <c r="AN117" s="6">
         <v>4.907617397534878</v>
       </c>
       <c r="AO117" s="6">
-        <v>1.2405919506742504</v>
+        <v>1.2405919506742449</v>
       </c>
       <c r="AP117" s="6">
-        <v>2.2796222724219146</v>
+        <v>2.2796222724219115</v>
       </c>
       <c r="AQ117" s="6">
-        <v>2.0231829492181856</v>
+        <v>2.0231829492181959</v>
       </c>
       <c r="AR117" s="6">
-        <v>1.0009433402463452</v>
+        <v>1.0009433402463301</v>
       </c>
       <c r="AS117" s="6">
-        <v>4.1388776941305263</v>
+        <v>4.1388776941305387</v>
       </c>
       <c r="AT117" s="6">
-        <v>3.1108292578039767</v>
+        <v>3.1108292578039811</v>
       </c>
       <c r="AU117" s="6">
-        <v>4.2781527662853804</v>
+        <v>4.2781527662853795</v>
       </c>
       <c r="AV117" s="6">
-        <v>-1.2970248935542317</v>
+        <v>-1.2970248935542221</v>
       </c>
       <c r="AW117" s="6">
-        <v>1.5928202735189203</v>
+        <v>1.5928202735189114</v>
       </c>
       <c r="AX117" s="6">
-        <v>4.78613136216015</v>
+        <v>4.7861313621601402</v>
       </c>
       <c r="AY117" s="6">
-        <v>1.4701581136548463</v>
+        <v>1.4701581136548509</v>
       </c>
       <c r="AZ117" s="6">
-        <v>2.9813994887245254</v>
+        <v>2.9813994887245285</v>
       </c>
       <c r="BA117" s="6">
-        <v>8.1155948153753688</v>
+        <v>8.1155948153753759</v>
       </c>
     </row>
     <row r="118" spans="1:53" x14ac:dyDescent="0.2">
@@ -20659,160 +20659,160 @@
         <v>42856</v>
       </c>
       <c r="B118" s="6">
-        <v>0.57694518514378756</v>
+        <v>0.57694518514379045</v>
       </c>
       <c r="C118" s="6">
-        <v>-1.0600160930915532</v>
+        <v>-1.0600160930915596</v>
       </c>
       <c r="D118" s="6">
-        <v>-1.6075479850134369</v>
+        <v>-1.6075479850134275</v>
       </c>
       <c r="E118" s="6">
-        <v>0.94512734775563556</v>
+        <v>0.94512734775564</v>
       </c>
       <c r="F118" s="6">
-        <v>1.094262422692573</v>
+        <v>1.0942624226925644</v>
       </c>
       <c r="G118" s="6">
-        <v>-0.86039056759906285</v>
+        <v>-0.86039056759905819</v>
       </c>
       <c r="H118" s="6">
-        <v>-2.6673732163624035</v>
+        <v>-2.667373216362384</v>
       </c>
       <c r="I118" s="6">
-        <v>-1.9842083154429868</v>
+        <v>-1.9842083154429737</v>
       </c>
       <c r="J118" s="6">
-        <v>-1.4679745653491656</v>
+        <v>-1.4679745653491623</v>
       </c>
       <c r="K118" s="6">
-        <v>-3.1987961003748273</v>
+        <v>-3.19879610037481</v>
       </c>
       <c r="L118" s="6">
-        <v>0.34699391284217318</v>
+        <v>0.34699391284218267</v>
       </c>
       <c r="M118" s="6">
-        <v>-1.5612847893747936</v>
+        <v>-1.5612847893747892</v>
       </c>
       <c r="N118" s="6">
-        <v>-2.6591087663233735</v>
+        <v>-2.6591087663233659</v>
       </c>
       <c r="O118" s="6">
-        <v>-2.3924445641195913</v>
+        <v>-2.3924445641195771</v>
       </c>
       <c r="P118" s="6">
-        <v>-3.5297843399034607</v>
+        <v>-3.5297843399034496</v>
       </c>
       <c r="Q118" s="6">
-        <v>2.3105091595455298</v>
+        <v>2.3105091595455223</v>
       </c>
       <c r="R118" s="6">
-        <v>-4.0546094321194044</v>
+        <v>-4.0546094321193911</v>
       </c>
       <c r="S118" s="6">
-        <v>-0.7634225174419188</v>
+        <v>-0.76342251744191458</v>
       </c>
       <c r="T118" s="6">
-        <v>0.29353195736472321</v>
+        <v>0.29353195736471882</v>
       </c>
       <c r="U118" s="6">
-        <v>-1.3821798647215138</v>
+        <v>-1.3821798647215096</v>
       </c>
       <c r="V118" s="6">
-        <v>2.9349602285822707</v>
+        <v>2.9349602285822742</v>
       </c>
       <c r="W118" s="6">
-        <v>-1.8403729778983666</v>
+        <v>-1.840372977898364</v>
       </c>
       <c r="X118" s="6">
-        <v>-0.74294197500664472</v>
+        <v>-0.74294197500663361</v>
       </c>
       <c r="Y118" s="6">
-        <v>1.0011714622100827</v>
+        <v>1.0011714622100834</v>
       </c>
       <c r="Z118" s="6">
-        <v>1.5441492465933844</v>
+        <v>1.5441492465933875</v>
       </c>
       <c r="AA118" s="6">
-        <v>-1.5955858780926191</v>
+        <v>-1.5955858780926127</v>
       </c>
       <c r="AB118" s="6">
-        <v>3.3029243344408203</v>
+        <v>3.3029243344408266</v>
       </c>
       <c r="AC118" s="6">
-        <v>-0.47903314978166406</v>
+        <v>-0.47903314978164901</v>
       </c>
       <c r="AD118" s="6">
-        <v>1.5617178041343653</v>
+        <v>1.5617178041343727</v>
       </c>
       <c r="AE118" s="6">
-        <v>-1.4884768020517221</v>
+        <v>-1.4884768020517303</v>
       </c>
       <c r="AF118" s="6">
-        <v>1.3663204418312322</v>
+        <v>1.3663204418312185</v>
       </c>
       <c r="AG118" s="6">
-        <v>2.9165668530277031</v>
+        <v>2.9165668530276898</v>
       </c>
       <c r="AH118" s="6">
-        <v>1.5311353016132558</v>
+        <v>1.5311353016132692</v>
       </c>
       <c r="AI118" s="6">
-        <v>-0.85089288244765826</v>
+        <v>-0.85089288244766115</v>
       </c>
       <c r="AJ118" s="6">
-        <v>8.6347758181857998E-2</v>
+        <v>8.6347758181848089E-2</v>
       </c>
       <c r="AK118" s="6">
         <v>-1.1637913952162751</v>
       </c>
       <c r="AL118" s="6">
-        <v>-0.70312062459373714</v>
+        <v>-0.70312062459373115</v>
       </c>
       <c r="AM118" s="6">
-        <v>1.8892218762125039</v>
+        <v>1.8892218762124986</v>
       </c>
       <c r="AN118" s="6">
-        <v>-2.54241448470595</v>
+        <v>-2.542414484705962</v>
       </c>
       <c r="AO118" s="6">
-        <v>-0.73178553407521374</v>
+        <v>-0.73178553407521607</v>
       </c>
       <c r="AP118" s="6">
-        <v>0.91705535085938661</v>
+        <v>0.91705535085938816</v>
       </c>
       <c r="AQ118" s="6">
-        <v>0.13809009893855589</v>
+        <v>0.13809009893854921</v>
       </c>
       <c r="AR118" s="6">
-        <v>-0.76272424492713764</v>
+        <v>-0.76272424492715207</v>
       </c>
       <c r="AS118" s="6">
-        <v>0.46858024403416026</v>
+        <v>0.46858024403416781</v>
       </c>
       <c r="AT118" s="6">
-        <v>-1.197110682947935</v>
+        <v>-1.1971106829479334</v>
       </c>
       <c r="AU118" s="6">
-        <v>-0.79646109436790868</v>
+        <v>-0.79646109436790924</v>
       </c>
       <c r="AV118" s="6">
-        <v>-2.3807317744357905</v>
+        <v>-2.3807317744357852</v>
       </c>
       <c r="AW118" s="6">
-        <v>-3.4782174333010847</v>
+        <v>-3.4782174333010798</v>
       </c>
       <c r="AX118" s="6">
-        <v>-1.6695839316119323</v>
+        <v>-1.6695839316119203</v>
       </c>
       <c r="AY118" s="6">
-        <v>2.8890633045695147</v>
+        <v>2.8890633045695187</v>
       </c>
       <c r="AZ118" s="6">
-        <v>-0.87262591996012628</v>
+        <v>-0.87262591996011807</v>
       </c>
       <c r="BA118" s="6">
-        <v>4.3798725383937631</v>
+        <v>4.3798725383937605</v>
       </c>
     </row>
     <row r="119" spans="1:53" x14ac:dyDescent="0.2">
@@ -20820,160 +20820,160 @@
         <v>42887</v>
       </c>
       <c r="B119" s="6">
-        <v>0.8499895100863144</v>
+        <v>0.8499895100863164</v>
       </c>
       <c r="C119" s="6">
-        <v>-0.60011986559530639</v>
+        <v>-0.60011986559529584</v>
       </c>
       <c r="D119" s="6">
         <v>1.5209754945034559</v>
       </c>
       <c r="E119" s="6">
-        <v>3.5982486069425099</v>
+        <v>3.5982486069425113</v>
       </c>
       <c r="F119" s="6">
-        <v>2.3787319936828579</v>
+        <v>2.3787319936828548</v>
       </c>
       <c r="G119" s="6">
-        <v>2.3403605948507917</v>
+        <v>2.3403605948507775</v>
       </c>
       <c r="H119" s="6">
-        <v>0.37954092854338706</v>
+        <v>0.37954092854338428</v>
       </c>
       <c r="I119" s="6">
-        <v>0.81715035937593505</v>
+        <v>0.81715035937595204</v>
       </c>
       <c r="J119" s="6">
-        <v>10.692171735391099</v>
+        <v>10.692171735391085</v>
       </c>
       <c r="K119" s="6">
-        <v>1.1303202298939543</v>
+        <v>1.1303202298939627</v>
       </c>
       <c r="L119" s="6">
-        <v>0.84789979889406519</v>
+        <v>0.84789979889405498</v>
       </c>
       <c r="M119" s="6">
-        <v>5.2287709853642967</v>
+        <v>5.2287709853642923</v>
       </c>
       <c r="N119" s="6">
-        <v>1.0934868443320938</v>
+        <v>1.0934868443320847</v>
       </c>
       <c r="O119" s="6">
-        <v>0.85645571946456023</v>
+        <v>0.85645571946455479</v>
       </c>
       <c r="P119" s="6">
-        <v>-0.81981149177344315</v>
+        <v>-0.81981149177345247</v>
       </c>
       <c r="Q119" s="6">
-        <v>4.3058163262613274</v>
+        <v>4.3058163262613292</v>
       </c>
       <c r="R119" s="6">
         <v>-4.5015266032705199</v>
       </c>
       <c r="S119" s="6">
-        <v>0.8962643207658797</v>
+        <v>0.89626432076588702</v>
       </c>
       <c r="T119" s="6">
-        <v>-8.7436501168156822E-2</v>
+        <v>-8.7436501168175251E-2</v>
       </c>
       <c r="U119" s="6">
-        <v>-5.3480665990868433E-2</v>
+        <v>-5.3480665990881908E-2</v>
       </c>
       <c r="V119" s="6">
-        <v>3.0900114373443697</v>
+        <v>3.0900114373443679</v>
       </c>
       <c r="W119" s="6">
-        <v>0.65632836746059386</v>
+        <v>0.65632836746058565</v>
       </c>
       <c r="X119" s="6">
-        <v>0.63787129069073156</v>
+        <v>0.63787129069072901</v>
       </c>
       <c r="Y119" s="6">
-        <v>1.6315032907431741</v>
+        <v>1.6315032907431553</v>
       </c>
       <c r="Z119" s="6">
-        <v>2.5922931041160195</v>
+        <v>2.5922931041160222</v>
       </c>
       <c r="AA119" s="6">
-        <v>0.63114316154130812</v>
+        <v>0.63114316154129024</v>
       </c>
       <c r="AB119" s="6">
-        <v>5.5418973399157334</v>
+        <v>5.5418973399157281</v>
       </c>
       <c r="AC119" s="6">
-        <v>1.7616268670368833</v>
+        <v>1.7616268670368715</v>
       </c>
       <c r="AD119" s="6">
-        <v>3.0113205354830912</v>
+        <v>3.011320535483097</v>
       </c>
       <c r="AE119" s="6">
-        <v>0.13802537444495175</v>
+        <v>0.13802537444495688</v>
       </c>
       <c r="AF119" s="6">
-        <v>2.4147059345470385</v>
+        <v>2.4147059345470256</v>
       </c>
       <c r="AG119" s="6">
-        <v>3.7900492529862295</v>
+        <v>3.7900492529862362</v>
       </c>
       <c r="AH119" s="6">
         <v>2.8217380111426182</v>
       </c>
       <c r="AI119" s="6">
-        <v>1.5794644258719823</v>
+        <v>1.5794644258719934</v>
       </c>
       <c r="AJ119" s="6">
-        <v>1.2530208443601198</v>
+        <v>1.253020844360111</v>
       </c>
       <c r="AK119" s="6">
-        <v>2.8670927127629713</v>
+        <v>2.8670927127629788</v>
       </c>
       <c r="AL119" s="6">
-        <v>1.0234296068980819</v>
+        <v>1.023429606898095</v>
       </c>
       <c r="AM119" s="6">
-        <v>3.6913838644023991</v>
+        <v>3.6913838644023902</v>
       </c>
       <c r="AN119" s="6">
-        <v>1.4667290010036158</v>
+        <v>1.4667290010036049</v>
       </c>
       <c r="AO119" s="6">
-        <v>0.50445478355403561</v>
+        <v>0.50445478355403328</v>
       </c>
       <c r="AP119" s="6">
-        <v>1.1098495934721322</v>
+        <v>1.1098495934721191</v>
       </c>
       <c r="AQ119" s="6">
-        <v>0.91050343737891726</v>
+        <v>0.91050343737890926</v>
       </c>
       <c r="AR119" s="6">
-        <v>0.21931025180177408</v>
+        <v>0.21931025180175484</v>
       </c>
       <c r="AS119" s="6">
-        <v>2.1399248634380861</v>
+        <v>2.139924863438099</v>
       </c>
       <c r="AT119" s="6">
-        <v>1.2666533124960677</v>
+        <v>1.2666533124960637</v>
       </c>
       <c r="AU119" s="6">
-        <v>2.7349995575736386</v>
+        <v>2.7349995575736408</v>
       </c>
       <c r="AV119" s="6">
-        <v>-1.6885382826227708</v>
+        <v>-1.6885382826227682</v>
       </c>
       <c r="AW119" s="6">
-        <v>-1.8253179992883475</v>
+        <v>-1.825317999288337</v>
       </c>
       <c r="AX119" s="6">
-        <v>1.9696124204740262</v>
+        <v>1.9696124204740282</v>
       </c>
       <c r="AY119" s="6">
-        <v>4.54749721948368</v>
+        <v>4.5474972194836889</v>
       </c>
       <c r="AZ119" s="6">
-        <v>0.60257924908621274</v>
+        <v>0.60257924908621507</v>
       </c>
       <c r="BA119" s="6">
-        <v>7.0744418491296033</v>
+        <v>7.0744418491296095</v>
       </c>
     </row>
     <row r="120" spans="1:53" x14ac:dyDescent="0.2">
@@ -20981,160 +20981,160 @@
         <v>42917</v>
       </c>
       <c r="B120" s="6">
-        <v>0.749790152605605</v>
+        <v>0.74979015260562609</v>
       </c>
       <c r="C120" s="6">
-        <v>0.37390569380318361</v>
+        <v>0.37390569380320604</v>
       </c>
       <c r="D120" s="6">
-        <v>0.48137017344345417</v>
+        <v>0.48137017344347893</v>
       </c>
       <c r="E120" s="6">
-        <v>8.4118268831580973</v>
+        <v>8.4118268831581098</v>
       </c>
       <c r="F120" s="6">
-        <v>1.7022307814358584</v>
+        <v>1.7022307814358639</v>
       </c>
       <c r="G120" s="6">
-        <v>5.5607722183231738</v>
+        <v>5.560772218323196</v>
       </c>
       <c r="H120" s="6">
-        <v>3.615433643216468</v>
+        <v>3.6154336432164791</v>
       </c>
       <c r="I120" s="6">
-        <v>2.1362951283689964</v>
+        <v>2.1362951283689844</v>
       </c>
       <c r="J120" s="6">
-        <v>11.066224348823575</v>
+        <v>11.066224348823598</v>
       </c>
       <c r="K120" s="6">
-        <v>6.6768689658067135</v>
+        <v>6.6768689658067437</v>
       </c>
       <c r="L120" s="6">
-        <v>3.8048191362976782</v>
+        <v>3.8048191362976969</v>
       </c>
       <c r="M120" s="6">
-        <v>7.0237606556998013</v>
+        <v>7.0237606556998244</v>
       </c>
       <c r="N120" s="6">
-        <v>4.8885970294876042</v>
+        <v>4.8885970294876149</v>
       </c>
       <c r="O120" s="6">
-        <v>3.4329296439494574</v>
+        <v>3.4329296439494903</v>
       </c>
       <c r="P120" s="6">
-        <v>1.1863003125104528</v>
+        <v>1.1863003125104636</v>
       </c>
       <c r="Q120" s="6">
-        <v>5.084577407833045</v>
+        <v>5.0845774078330761</v>
       </c>
       <c r="R120" s="6">
-        <v>-1.7605352989037457</v>
+        <v>-1.7605352989037335</v>
       </c>
       <c r="S120" s="6">
-        <v>2.7132198874243736</v>
+        <v>2.7132198874243909</v>
       </c>
       <c r="T120" s="6">
-        <v>1.828994456420284</v>
+        <v>1.8289944564202989</v>
       </c>
       <c r="U120" s="6">
-        <v>2.8478430980444931</v>
+        <v>2.8478430980445104</v>
       </c>
       <c r="V120" s="6">
-        <v>3.8854147697349575</v>
+        <v>3.8854147697349539</v>
       </c>
       <c r="W120" s="6">
-        <v>2.8576192271672145</v>
+        <v>2.8576192271672194</v>
       </c>
       <c r="X120" s="6">
-        <v>1.9833216143932964</v>
+        <v>1.9833216143933357</v>
       </c>
       <c r="Y120" s="6">
-        <v>2.110696819671948</v>
+        <v>2.1106968196719675</v>
       </c>
       <c r="Z120" s="6">
-        <v>4.5749050577517103</v>
+        <v>4.5749050577517156</v>
       </c>
       <c r="AA120" s="6">
-        <v>1.2204384731435962</v>
+        <v>1.220438473143622</v>
       </c>
       <c r="AB120" s="6">
-        <v>7.8459247525013556</v>
+        <v>7.8459247525013751</v>
       </c>
       <c r="AC120" s="6">
-        <v>3.1874579961821699</v>
+        <v>3.1874579961821929</v>
       </c>
       <c r="AD120" s="6">
-        <v>4.8599896367134976</v>
+        <v>4.8599896367134994</v>
       </c>
       <c r="AE120" s="6">
-        <v>1.9047499961891197</v>
+        <v>1.9047499961891399</v>
       </c>
       <c r="AF120" s="6">
-        <v>0.7728045350556404</v>
+        <v>0.77280453505565982</v>
       </c>
       <c r="AG120" s="6">
-        <v>4.0044902832399538</v>
+        <v>4.0044902832399805</v>
       </c>
       <c r="AH120" s="6">
-        <v>4.307929896527452</v>
+        <v>4.3079298965274795</v>
       </c>
       <c r="AI120" s="6">
-        <v>2.4368410671557217</v>
+        <v>2.4368410671557497</v>
       </c>
       <c r="AJ120" s="6">
-        <v>3.2423894886317384</v>
+        <v>3.2423894886317584</v>
       </c>
       <c r="AK120" s="6">
-        <v>3.5329849319689908</v>
+        <v>3.5329849319690076</v>
       </c>
       <c r="AL120" s="6">
-        <v>2.222519929714228</v>
+        <v>2.2225199297142524</v>
       </c>
       <c r="AM120" s="6">
-        <v>5.1969639854585621</v>
+        <v>5.1969639854585754</v>
       </c>
       <c r="AN120" s="6">
-        <v>3.1567534055491011</v>
+        <v>3.1567534055491198</v>
       </c>
       <c r="AO120" s="6">
-        <v>0.37030358753345477</v>
+        <v>0.37030358753347231</v>
       </c>
       <c r="AP120" s="6">
-        <v>3.1183530170192242</v>
+        <v>3.1183530170192357</v>
       </c>
       <c r="AQ120" s="6">
-        <v>3.7077600406370572</v>
+        <v>3.7077600406370799</v>
       </c>
       <c r="AR120" s="6">
-        <v>0.42531867319857131</v>
+        <v>0.42531867319859112</v>
       </c>
       <c r="AS120" s="6">
-        <v>2.6965136817309525</v>
+        <v>2.6965136817309689</v>
       </c>
       <c r="AT120" s="6">
-        <v>4.6664867241493546</v>
+        <v>4.6664867241493653</v>
       </c>
       <c r="AU120" s="6">
-        <v>5.459240442949997</v>
+        <v>5.4592404429500148</v>
       </c>
       <c r="AV120" s="6">
-        <v>-0.33571054636611125</v>
+        <v>-0.3357105463661027</v>
       </c>
       <c r="AW120" s="6">
-        <v>8.3271452618222011E-2</v>
+        <v>8.3271452618217973E-2</v>
       </c>
       <c r="AX120" s="6">
-        <v>5.3250625850395146</v>
+        <v>5.3250625850395066</v>
       </c>
       <c r="AY120" s="6">
-        <v>4.4858172573508739</v>
+        <v>4.4858172573509023</v>
       </c>
       <c r="AZ120" s="6">
-        <v>1.83116777655675</v>
+        <v>1.8311677765567753</v>
       </c>
       <c r="BA120" s="6">
-        <v>7.7026008821686878</v>
+        <v>7.7026008821687082</v>
       </c>
     </row>
     <row r="121" spans="1:53" x14ac:dyDescent="0.2">
@@ -21142,160 +21142,160 @@
         <v>42948</v>
       </c>
       <c r="B121" s="6">
-        <v>0.94677151042636787</v>
+        <v>0.94677151042637331</v>
       </c>
       <c r="C121" s="6">
-        <v>0.83087148763981744</v>
+        <v>0.83087148763983198</v>
       </c>
       <c r="D121" s="6">
-        <v>0.62758115877068066</v>
+        <v>0.62758115877069609</v>
       </c>
       <c r="E121" s="6">
-        <v>5.5070533983758017</v>
+        <v>5.5070533983758034</v>
       </c>
       <c r="F121" s="6">
-        <v>2.2560953240584993</v>
+        <v>2.2560953240585122</v>
       </c>
       <c r="G121" s="6">
-        <v>2.1914996104725817</v>
+        <v>2.1914996104725843</v>
       </c>
       <c r="H121" s="6">
-        <v>1.2697115645203145</v>
+        <v>1.2697115645203174</v>
       </c>
       <c r="I121" s="6">
-        <v>7.8887041551145426E-2</v>
+        <v>7.8887041551145246E-2</v>
       </c>
       <c r="J121" s="6">
-        <v>7.6956278017020594</v>
+        <v>7.6956278017020709</v>
       </c>
       <c r="K121" s="6">
-        <v>0.56684964678562</v>
+        <v>0.56684964678562189</v>
       </c>
       <c r="L121" s="6">
-        <v>1.8077787113395745</v>
+        <v>1.8077787113395836</v>
       </c>
       <c r="M121" s="6">
-        <v>5.3456028934462694</v>
+        <v>5.3456028934462729</v>
       </c>
       <c r="N121" s="6">
-        <v>1.7270961544708905</v>
+        <v>1.727096154470896</v>
       </c>
       <c r="O121" s="6">
-        <v>1.0966726001660034</v>
+        <v>1.0966726001660119</v>
       </c>
       <c r="P121" s="6">
-        <v>-0.85044597000593203</v>
+        <v>-0.85044597000592626</v>
       </c>
       <c r="Q121" s="6">
-        <v>3.8002102060623293</v>
+        <v>3.8002102060623448</v>
       </c>
       <c r="R121" s="6">
-        <v>-2.3991902571647095</v>
+        <v>-2.3991902571647112</v>
       </c>
       <c r="S121" s="6">
-        <v>0.65142605154762245</v>
+        <v>0.651426051547634</v>
       </c>
       <c r="T121" s="6">
-        <v>1.7465815652508498</v>
+        <v>1.7465815652508578</v>
       </c>
       <c r="U121" s="6">
-        <v>2.3263631922049344</v>
+        <v>2.326363192204945</v>
       </c>
       <c r="V121" s="6">
         <v>3.3480696111277277</v>
       </c>
       <c r="W121" s="6">
-        <v>-0.40711022434835703</v>
+        <v>-0.40711022434834193</v>
       </c>
       <c r="X121" s="6">
-        <v>0.61929733633756268</v>
+        <v>0.61929733633756445</v>
       </c>
       <c r="Y121" s="6">
-        <v>1.112168471884426</v>
+        <v>1.1121684718844305</v>
       </c>
       <c r="Z121" s="6">
-        <v>3.2167937445717674</v>
+        <v>3.2167937445717762</v>
       </c>
       <c r="AA121" s="6">
-        <v>1.4840810379588818</v>
+        <v>1.4840810379588931</v>
       </c>
       <c r="AB121" s="6">
-        <v>6.0898242921157575</v>
+        <v>6.089824292115753</v>
       </c>
       <c r="AC121" s="6">
-        <v>1.6035384761854892</v>
+        <v>1.6035384761854996</v>
       </c>
       <c r="AD121" s="6">
-        <v>2.5827476110358951</v>
+        <v>2.5827476110359036</v>
       </c>
       <c r="AE121" s="6">
-        <v>-0.19108311325689753</v>
+        <v>-0.19108311325689978</v>
       </c>
       <c r="AF121" s="6">
-        <v>-0.17980329435206835</v>
+        <v>-0.17980329435206549</v>
       </c>
       <c r="AG121" s="6">
-        <v>2.2556426995515784</v>
+        <v>2.255642699551585</v>
       </c>
       <c r="AH121" s="6">
-        <v>1.8343318890050582</v>
+        <v>1.8343318890050622</v>
       </c>
       <c r="AI121" s="6">
-        <v>-1.614531886630582</v>
+        <v>-1.6145318866305867</v>
       </c>
       <c r="AJ121" s="6">
-        <v>0.27345549473258163</v>
+        <v>0.27345549473258829</v>
       </c>
       <c r="AK121" s="6">
-        <v>1.7782326236769384</v>
+        <v>1.7782326236769526</v>
       </c>
       <c r="AL121" s="6">
-        <v>1.095790933473421</v>
+        <v>1.0957909334734117</v>
       </c>
       <c r="AM121" s="6">
-        <v>3.9910662685136558</v>
+        <v>3.9910662685136669</v>
       </c>
       <c r="AN121" s="6">
-        <v>1.0484121703976574</v>
+        <v>1.0484121703976774</v>
       </c>
       <c r="AO121" s="6">
-        <v>-0.16756414632088551</v>
+        <v>-0.16756414632087957</v>
       </c>
       <c r="AP121" s="6">
-        <v>1.7046164939081005</v>
+        <v>1.7046164939081054</v>
       </c>
       <c r="AQ121" s="6">
-        <v>2.5384780241208533</v>
+        <v>2.5384780241208631</v>
       </c>
       <c r="AR121" s="6">
-        <v>-0.32551231997080116</v>
+        <v>-0.32551231997079588</v>
       </c>
       <c r="AS121" s="6">
-        <v>1.0763177262985928</v>
+        <v>1.0763177262986037</v>
       </c>
       <c r="AT121" s="6">
-        <v>1.5152819756369444</v>
+        <v>1.5152819756369627</v>
       </c>
       <c r="AU121" s="6">
-        <v>3.0890122285423991</v>
+        <v>3.089012228542404</v>
       </c>
       <c r="AV121" s="6">
-        <v>-2.5132397850706036E-3</v>
+        <v>-2.5132397850542048E-3</v>
       </c>
       <c r="AW121" s="6">
-        <v>-2.050017366494906</v>
+        <v>-2.0500173664948989</v>
       </c>
       <c r="AX121" s="6">
-        <v>1.9173080541767746</v>
+        <v>1.9173080541767953</v>
       </c>
       <c r="AY121" s="6">
-        <v>3.9396200878675209</v>
+        <v>3.9396200878675289</v>
       </c>
       <c r="AZ121" s="6">
-        <v>0.36293725125910586</v>
+        <v>0.36293725125910159</v>
       </c>
       <c r="BA121" s="6">
-        <v>3.4290516581644401</v>
+        <v>3.4290516581644606</v>
       </c>
     </row>
     <row r="122" spans="1:53" x14ac:dyDescent="0.2">
@@ -21303,160 +21303,160 @@
         <v>42979</v>
       </c>
       <c r="B122" s="6">
-        <v>0.29310732651880089</v>
+        <v>0.29310732651879562</v>
       </c>
       <c r="C122" s="6">
-        <v>0.32210119112057334</v>
+        <v>0.32210119112056579</v>
       </c>
       <c r="D122" s="6">
-        <v>9.8859913492484949E-2</v>
+        <v>9.8859913492480259E-2</v>
       </c>
       <c r="E122" s="6">
-        <v>5.0871831190632193</v>
+        <v>5.0871831190632273</v>
       </c>
       <c r="F122" s="6">
-        <v>3.8951836043709562</v>
+        <v>3.8951836043709442</v>
       </c>
       <c r="G122" s="6">
-        <v>2.1728468464195281</v>
+        <v>2.1728468464195192</v>
       </c>
       <c r="H122" s="6">
-        <v>0.90600736708759677</v>
+        <v>0.90600736708758189</v>
       </c>
       <c r="I122" s="6">
-        <v>-0.18775683558579576</v>
+        <v>-0.18775683558580886</v>
       </c>
       <c r="J122" s="6">
         <v>7.1915220311454515</v>
       </c>
       <c r="K122" s="6">
-        <v>1.4799760221476359</v>
+        <v>1.4799760221476399</v>
       </c>
       <c r="L122" s="6">
-        <v>0.24859460086798488</v>
+        <v>0.24859460086796725</v>
       </c>
       <c r="M122" s="6">
-        <v>4.1236418589548958</v>
+        <v>4.1236418589548931</v>
       </c>
       <c r="N122" s="6">
-        <v>2.3483159516169736</v>
+        <v>2.3483159516169581</v>
       </c>
       <c r="O122" s="6">
-        <v>1.1499083860837165</v>
+        <v>1.1499083860837005</v>
       </c>
       <c r="P122" s="6">
-        <v>-0.7933437621370184</v>
+        <v>-0.79334376213702784</v>
       </c>
       <c r="Q122" s="6">
-        <v>3.2550342477454133</v>
+        <v>3.255034247745392</v>
       </c>
       <c r="R122" s="6">
-        <v>-1.9439235664286709</v>
+        <v>-1.9439235664286796</v>
       </c>
       <c r="S122" s="6">
-        <v>0.6642976138415041</v>
+        <v>0.66429761384148067</v>
       </c>
       <c r="T122" s="6">
-        <v>0.67213701219520883</v>
+        <v>0.67213701219518851</v>
       </c>
       <c r="U122" s="6">
-        <v>0.15041688124371658</v>
+        <v>0.15041688124370875</v>
       </c>
       <c r="V122" s="6">
-        <v>2.8240929129316199</v>
+        <v>2.8240929129316106</v>
       </c>
       <c r="W122" s="6">
-        <v>3.3737956959640205</v>
+        <v>3.3737956959640174</v>
       </c>
       <c r="X122" s="6">
-        <v>0.48863122834953077</v>
+        <v>0.48863122834952266</v>
       </c>
       <c r="Y122" s="6">
-        <v>1.3848416138460704</v>
+        <v>1.3848416138460669</v>
       </c>
       <c r="Z122" s="6">
-        <v>2.3275088258466368</v>
+        <v>2.3275088258466328</v>
       </c>
       <c r="AA122" s="6">
-        <v>1.1390691253065042</v>
+        <v>1.1390691253065026</v>
       </c>
       <c r="AB122" s="6">
-        <v>4.2163670152909161</v>
+        <v>4.2163670152909107</v>
       </c>
       <c r="AC122" s="6">
-        <v>1.1083849731451936</v>
+        <v>1.108384973145176</v>
       </c>
       <c r="AD122" s="6">
-        <v>3.5862696475870508</v>
+        <v>3.5862696475870321</v>
       </c>
       <c r="AE122" s="6">
-        <v>-7.4095356975890014E-3</v>
+        <v>-7.4095356975917969E-3</v>
       </c>
       <c r="AF122" s="6">
-        <v>-0.50795617955746719</v>
+        <v>-0.50795617955746519</v>
       </c>
       <c r="AG122" s="6">
-        <v>-0.48813667051013199</v>
+        <v>-0.48813667051014442</v>
       </c>
       <c r="AH122" s="6">
-        <v>0.9339338228494859</v>
+        <v>0.93393382284947601</v>
       </c>
       <c r="AI122" s="6">
-        <v>0.19922377847487346</v>
+        <v>0.19922377847484732</v>
       </c>
       <c r="AJ122" s="6">
-        <v>0.85265064641281796</v>
+        <v>0.85265064641281829</v>
       </c>
       <c r="AK122" s="6">
-        <v>0.9806019292249406</v>
+        <v>0.98060192922493195</v>
       </c>
       <c r="AL122" s="6">
-        <v>0.39124308592774726</v>
+        <v>0.39124308592773627</v>
       </c>
       <c r="AM122" s="6">
-        <v>2.4269798331209387</v>
+        <v>2.4269798331209178</v>
       </c>
       <c r="AN122" s="6">
-        <v>0.61282714495392276</v>
+        <v>0.61282714495390911</v>
       </c>
       <c r="AO122" s="6">
-        <v>0.19802629285925782</v>
+        <v>0.19802629285923914</v>
       </c>
       <c r="AP122" s="6">
-        <v>3.207928960339236</v>
+        <v>3.2079289603392138</v>
       </c>
       <c r="AQ122" s="6">
-        <v>0.50329467511254034</v>
+        <v>0.50329467511252213</v>
       </c>
       <c r="AR122" s="6">
-        <v>-1.7446207769886073</v>
+        <v>-1.7446207769886177</v>
       </c>
       <c r="AS122" s="6">
-        <v>0.52141319264910491</v>
+        <v>0.52141319264909636</v>
       </c>
       <c r="AT122" s="6">
-        <v>2.3719886056136916</v>
+        <v>2.3719886056136903</v>
       </c>
       <c r="AU122" s="6">
-        <v>1.7587747144880039</v>
+        <v>1.7587747144879859</v>
       </c>
       <c r="AV122" s="6">
-        <v>-1.3396701744013977</v>
+        <v>-1.3396701744014041</v>
       </c>
       <c r="AW122" s="6">
-        <v>-2.1533190257049957</v>
+        <v>-2.1533190257050157</v>
       </c>
       <c r="AX122" s="6">
-        <v>1.511229068562248</v>
+        <v>1.5112290685622227</v>
       </c>
       <c r="AY122" s="6">
-        <v>3.7877069257807956</v>
+        <v>3.7877069257807823</v>
       </c>
       <c r="AZ122" s="6">
-        <v>2.6503041786915782</v>
+        <v>2.650304178691568</v>
       </c>
       <c r="BA122" s="6">
-        <v>4.0342266701153005</v>
+        <v>4.0342266701152916</v>
       </c>
     </row>
     <row r="123" spans="1:53" x14ac:dyDescent="0.2">
@@ -21464,160 +21464,160 @@
         <v>43009</v>
       </c>
       <c r="B123" s="6">
-        <v>0.23429614042852054</v>
+        <v>0.23429614042853411</v>
       </c>
       <c r="C123" s="6">
-        <v>4.6560146508501182E-2</v>
+        <v>4.6560146508526114E-2</v>
       </c>
       <c r="D123" s="6">
-        <v>-0.51269583036348687</v>
+        <v>-0.51269583036348998</v>
       </c>
       <c r="E123" s="6">
-        <v>5.1064029206831387</v>
+        <v>5.1064029206831538</v>
       </c>
       <c r="F123" s="6">
-        <v>1.9410601596321544</v>
+        <v>1.9410601596321793</v>
       </c>
       <c r="G123" s="6">
-        <v>1.6992832646771265</v>
+        <v>1.6992832646771558</v>
       </c>
       <c r="H123" s="6">
-        <v>-0.32771680985117152</v>
+        <v>-0.32771680985116747</v>
       </c>
       <c r="I123" s="6">
-        <v>-0.6448638568013213</v>
+        <v>-0.64486385680130909</v>
       </c>
       <c r="J123" s="6">
-        <v>2.5564205658200354</v>
+        <v>2.5564205658200359</v>
       </c>
       <c r="K123" s="6">
-        <v>1.7211564703469184</v>
+        <v>1.7211564703469289</v>
       </c>
       <c r="L123" s="6">
-        <v>2.2314585484092957</v>
+        <v>2.2314585484093139</v>
       </c>
       <c r="M123" s="6">
-        <v>4.2941756610065926</v>
+        <v>4.2941756610066095</v>
       </c>
       <c r="N123" s="6">
-        <v>2.1669945063068679</v>
+        <v>2.1669945063068692</v>
       </c>
       <c r="O123" s="6">
-        <v>0.9064214478234025</v>
+        <v>0.90642144782341705</v>
       </c>
       <c r="P123" s="6">
-        <v>-1.3827872135407362</v>
+        <v>-1.3827872135407246</v>
       </c>
       <c r="Q123" s="6">
-        <v>1.2969056052586923</v>
+        <v>1.2969056052587111</v>
       </c>
       <c r="R123" s="6">
-        <v>-3.478628872652028</v>
+        <v>-3.4786288726520094</v>
       </c>
       <c r="S123" s="6">
-        <v>-0.56224693648387591</v>
+        <v>-0.5622469364838617</v>
       </c>
       <c r="T123" s="6">
-        <v>-1.0522514693656164</v>
+        <v>-1.0522514693656049</v>
       </c>
       <c r="U123" s="6">
-        <v>-1.3654079379287107</v>
+        <v>-1.3654079379287143</v>
       </c>
       <c r="V123" s="6">
-        <v>1.3534849631306312</v>
+        <v>1.3534849631306494</v>
       </c>
       <c r="W123" s="6">
-        <v>4.1523529162762118</v>
+        <v>4.1523529162762491</v>
       </c>
       <c r="X123" s="6">
-        <v>-0.35611672154879287</v>
+        <v>-0.35611672154876922</v>
       </c>
       <c r="Y123" s="6">
-        <v>1.0647842418957814</v>
+        <v>1.0647842418957998</v>
       </c>
       <c r="Z123" s="6">
-        <v>1.7470134368957038</v>
+        <v>1.7470134368957064</v>
       </c>
       <c r="AA123" s="6">
-        <v>-1.1077509124735436</v>
+        <v>-1.1077509124735245</v>
       </c>
       <c r="AB123" s="6">
-        <v>2.8682247186509651</v>
+        <v>2.8682247186509753</v>
       </c>
       <c r="AC123" s="6">
-        <v>1.2241304403740614</v>
+        <v>1.2241304403740578</v>
       </c>
       <c r="AD123" s="6">
-        <v>3.2031270817635611</v>
+        <v>3.2031270817635717</v>
       </c>
       <c r="AE123" s="6">
-        <v>7.5108187115970892E-2</v>
+        <v>7.5108187115976471E-2</v>
       </c>
       <c r="AF123" s="6">
-        <v>-3.4793292251428736</v>
+        <v>-3.4793292251428625</v>
       </c>
       <c r="AG123" s="6">
-        <v>-0.97954068223668544</v>
+        <v>-0.97954068223667679</v>
       </c>
       <c r="AH123" s="6">
-        <v>0.69587555009681612</v>
+        <v>0.69587555009682112</v>
       </c>
       <c r="AI123" s="6">
-        <v>0.87728124384471862</v>
+        <v>0.87728124384472106</v>
       </c>
       <c r="AJ123" s="6">
-        <v>1.4617556872579092</v>
+        <v>1.4617556872579247</v>
       </c>
       <c r="AK123" s="6">
-        <v>-0.24737257039722732</v>
+        <v>-0.24737257039722421</v>
       </c>
       <c r="AL123" s="6">
-        <v>-0.19285572234741524</v>
+        <v>-0.19285572234740389</v>
       </c>
       <c r="AM123" s="6">
-        <v>1.9430139496360144</v>
+        <v>1.9430139496360168</v>
       </c>
       <c r="AN123" s="6">
-        <v>0.10588823817536111</v>
+        <v>0.10588823817537406</v>
       </c>
       <c r="AO123" s="6">
-        <v>-0.78667076442665052</v>
+        <v>-0.78667076442663975</v>
       </c>
       <c r="AP123" s="6">
-        <v>3.8411903974213137</v>
+        <v>3.8411903974213271</v>
       </c>
       <c r="AQ123" s="6">
-        <v>2.5071291259337944</v>
+        <v>2.507129125933798</v>
       </c>
       <c r="AR123" s="6">
-        <v>-1.688020118335851</v>
+        <v>-1.6880201183358381</v>
       </c>
       <c r="AS123" s="6">
-        <v>-1.3552579731957828</v>
+        <v>-1.3552579731957715</v>
       </c>
       <c r="AT123" s="6">
-        <v>1.4918725934342572</v>
+        <v>1.4918725934342687</v>
       </c>
       <c r="AU123" s="6">
-        <v>2.5900680912351679</v>
+        <v>2.5900680912351857</v>
       </c>
       <c r="AV123" s="6">
-        <v>-1.2301206757084417</v>
+        <v>-1.2301206757084211</v>
       </c>
       <c r="AW123" s="6">
-        <v>-2.47794424620146</v>
+        <v>-2.4779442462014489</v>
       </c>
       <c r="AX123" s="6">
-        <v>1.4303041864308979</v>
+        <v>1.4303041864309021</v>
       </c>
       <c r="AY123" s="6">
-        <v>3.2632447076794051</v>
+        <v>3.26324470767943</v>
       </c>
       <c r="AZ123" s="6">
-        <v>2.0525512382090381</v>
+        <v>2.052551238209039</v>
       </c>
       <c r="BA123" s="6">
-        <v>3.3728245014003004</v>
+        <v>3.3728245014003138</v>
       </c>
     </row>
     <row r="124" spans="1:53" x14ac:dyDescent="0.2">
@@ -21625,160 +21625,160 @@
         <v>43040</v>
       </c>
       <c r="B124" s="6">
-        <v>0.84729592675504184</v>
+        <v>0.84729592675504595</v>
       </c>
       <c r="C124" s="6">
-        <v>1.1298152683838971</v>
+        <v>1.1298152683838891</v>
       </c>
       <c r="D124" s="6">
-        <v>-0.19530029659376949</v>
+        <v>-0.19530029659376982</v>
       </c>
       <c r="E124" s="6">
-        <v>5.020851298547667</v>
+        <v>5.0208512985476581</v>
       </c>
       <c r="F124" s="6">
         <v>2.1198465292159594</v>
       </c>
       <c r="G124" s="6">
-        <v>1.8918665114456907</v>
+        <v>1.8918665114456672</v>
       </c>
       <c r="H124" s="6">
-        <v>1.668908714300132</v>
+        <v>1.6689087143001373</v>
       </c>
       <c r="I124" s="6">
-        <v>-5.7102193031303539E-2</v>
+        <v>-5.7102193031319824E-2</v>
       </c>
       <c r="J124" s="6">
-        <v>3.2177530569288839</v>
+        <v>3.2177530569288813</v>
       </c>
       <c r="K124" s="6">
-        <v>1.2318370024955247</v>
+        <v>1.2318370024955412</v>
       </c>
       <c r="L124" s="6">
-        <v>2.003043846353568</v>
+        <v>2.0030438463535862</v>
       </c>
       <c r="M124" s="6">
-        <v>3.8837064543970414</v>
+        <v>3.8837064543970348</v>
       </c>
       <c r="N124" s="6">
-        <v>5.0094023467163993</v>
+        <v>5.0094023467164037</v>
       </c>
       <c r="O124" s="6">
-        <v>0.88785386116615761</v>
+        <v>0.88785386116614817</v>
       </c>
       <c r="P124" s="6">
-        <v>-0.14721841279546877</v>
+        <v>-0.14721841279547085</v>
       </c>
       <c r="Q124" s="6">
-        <v>1.7767269261296754</v>
+        <v>1.776726926129667</v>
       </c>
       <c r="R124" s="6">
-        <v>-0.98483371892629046</v>
+        <v>-0.98483371892628613</v>
       </c>
       <c r="S124" s="6">
-        <v>-3.2591800023434895E-3</v>
+        <v>-3.2591800023362301E-3</v>
       </c>
       <c r="T124" s="6">
-        <v>-1.2134242961462176</v>
+        <v>-1.2134242961462203</v>
       </c>
       <c r="U124" s="6">
-        <v>-0.41332611219779131</v>
+        <v>-0.41332611219779336</v>
       </c>
       <c r="V124" s="6">
-        <v>2.030762694982152</v>
+        <v>2.0307626949821542</v>
       </c>
       <c r="W124" s="6">
-        <v>4.2307008222223033</v>
+        <v>4.2307008222222988</v>
       </c>
       <c r="X124" s="6">
-        <v>0.9859434023038639</v>
+        <v>0.9859434023038316</v>
       </c>
       <c r="Y124" s="6">
-        <v>1.2148815387250873</v>
+        <v>1.2148815387250897</v>
       </c>
       <c r="Z124" s="6">
-        <v>0.22695012547245852</v>
+        <v>0.22695012547246349</v>
       </c>
       <c r="AA124" s="6">
-        <v>4.8579987144207776E-2</v>
+        <v>4.8579987144190276E-2</v>
       </c>
       <c r="AB124" s="6">
-        <v>2.82845683360526</v>
+        <v>2.8284568336052538</v>
       </c>
       <c r="AC124" s="6">
-        <v>1.0739888872539776</v>
+        <v>1.0739888872539725</v>
       </c>
       <c r="AD124" s="6">
-        <v>6.4218272940475334</v>
+        <v>6.4218272940475387</v>
       </c>
       <c r="AE124" s="6">
-        <v>0.59992007030735994</v>
+        <v>0.59992007030736072</v>
       </c>
       <c r="AF124" s="6">
-        <v>-2.2746705242252476</v>
+        <v>-2.274670524225249</v>
       </c>
       <c r="AG124" s="6">
-        <v>6.3157167594525845E-2</v>
+        <v>6.3157167594548785E-2</v>
       </c>
       <c r="AH124" s="6">
-        <v>1.9937154053242649</v>
+        <v>1.9937154053242676</v>
       </c>
       <c r="AI124" s="6">
-        <v>0.77935316562218526</v>
+        <v>0.77935316562217605</v>
       </c>
       <c r="AJ124" s="6">
-        <v>-4.9314585492345964E-2</v>
+        <v>-4.9314585492342647E-2</v>
       </c>
       <c r="AK124" s="6">
-        <v>2.0392417115175703</v>
+        <v>2.0392417115175641</v>
       </c>
       <c r="AL124" s="6">
-        <v>3.2737593995003131E-2</v>
+        <v>3.2737593994999301E-2</v>
       </c>
       <c r="AM124" s="6">
-        <v>1.6061723223923252</v>
+        <v>1.6061723223923212</v>
       </c>
       <c r="AN124" s="6">
-        <v>-0.33708186703161414</v>
+        <v>-0.33708186703161824</v>
       </c>
       <c r="AO124" s="6">
-        <v>-0.49529072304111954</v>
+        <v>-0.49529072304112426</v>
       </c>
       <c r="AP124" s="6">
-        <v>4.337634477341985</v>
+        <v>4.3376344773419957</v>
       </c>
       <c r="AQ124" s="6">
-        <v>1.0365621797305176</v>
+        <v>1.0365621797305078</v>
       </c>
       <c r="AR124" s="6">
-        <v>-2.4399789338482307</v>
+        <v>-2.4399789338482218</v>
       </c>
       <c r="AS124" s="6">
-        <v>-0.12024903483601553</v>
+        <v>-0.12024903483601579</v>
       </c>
       <c r="AT124" s="6">
-        <v>2.3443824456896705</v>
+        <v>2.3443824456896767</v>
       </c>
       <c r="AU124" s="6">
-        <v>0.68122925485233554</v>
+        <v>0.68122925485233321</v>
       </c>
       <c r="AV124" s="6">
-        <v>-1.7978036318821693</v>
+        <v>-1.7978036318821773</v>
       </c>
       <c r="AW124" s="6">
-        <v>-1.7841300650699727</v>
+        <v>-1.7841300650699716</v>
       </c>
       <c r="AX124" s="6">
-        <v>1.4272897065337951</v>
+        <v>1.4272897065337906</v>
       </c>
       <c r="AY124" s="6">
-        <v>3.3307040393798752</v>
+        <v>3.3307040393798735</v>
       </c>
       <c r="AZ124" s="6">
-        <v>1.8267570536746376</v>
+        <v>1.8267570536746578</v>
       </c>
       <c r="BA124" s="6">
-        <v>3.001725878441599</v>
+        <v>3.0017258784415879</v>
       </c>
     </row>
     <row r="125" spans="1:53" x14ac:dyDescent="0.2">
@@ -21786,160 +21786,160 @@
         <v>43070</v>
       </c>
       <c r="B125" s="6">
-        <v>0.83078238527232906</v>
+        <v>0.83078238527233317</v>
       </c>
       <c r="C125" s="6">
-        <v>1.7975588656525272</v>
+        <v>1.7975588656525205</v>
       </c>
       <c r="D125" s="6">
-        <v>0.93467086232280461</v>
+        <v>0.93467086232279106</v>
       </c>
       <c r="E125" s="6">
-        <v>5.2506361624097009</v>
+        <v>5.2506361624096929</v>
       </c>
       <c r="F125" s="6">
-        <v>3.1838275799008282</v>
+        <v>3.1838275799008469</v>
       </c>
       <c r="G125" s="6">
-        <v>1.617745393092054</v>
+        <v>1.6177453930920502</v>
       </c>
       <c r="H125" s="6">
-        <v>2.8397134799185317</v>
+        <v>2.8397134799185237</v>
       </c>
       <c r="I125" s="6">
-        <v>0.48227132450581867</v>
+        <v>0.48227132450582083</v>
       </c>
       <c r="J125" s="6">
-        <v>4.60681627543853</v>
+        <v>4.6068162754385344</v>
       </c>
       <c r="K125" s="6">
-        <v>1.6583152309082139</v>
+        <v>1.6583152309082128</v>
       </c>
       <c r="L125" s="6">
-        <v>2.5470791623327038</v>
+        <v>2.5470791623327047</v>
       </c>
       <c r="M125" s="6">
-        <v>3.7568572876501145</v>
+        <v>3.7568572876501118</v>
       </c>
       <c r="N125" s="6">
-        <v>4.7688223403239096</v>
+        <v>4.7688223403239025</v>
       </c>
       <c r="O125" s="6">
-        <v>2.6487289552493736</v>
+        <v>2.6487289552493589</v>
       </c>
       <c r="P125" s="6">
-        <v>0.46782858907344282</v>
+        <v>0.46782858907344133</v>
       </c>
       <c r="Q125" s="6">
-        <v>3.5931098844238964</v>
+        <v>3.5931098844238827</v>
       </c>
       <c r="R125" s="6">
-        <v>0.99803913544774281</v>
+        <v>0.99803913544774181</v>
       </c>
       <c r="S125" s="6">
-        <v>1.3234522706286678</v>
+        <v>1.3234522706286611</v>
       </c>
       <c r="T125" s="6">
-        <v>-1.6257990147011327</v>
+        <v>-1.6257990147011439</v>
       </c>
       <c r="U125" s="6">
-        <v>-0.47394046587826233</v>
+        <v>-0.47394046587825955</v>
       </c>
       <c r="V125" s="6">
-        <v>2.8630103125136772</v>
+        <v>2.8630103125136723</v>
       </c>
       <c r="W125" s="6">
-        <v>4.5128526401509479</v>
+        <v>4.512852640150947</v>
       </c>
       <c r="X125" s="6">
-        <v>0.42935174369704299</v>
+        <v>0.42935174369701207</v>
       </c>
       <c r="Y125" s="6">
-        <v>2.3073998685415553</v>
+        <v>2.3073998685415562</v>
       </c>
       <c r="Z125" s="6">
-        <v>0.81716461063345658</v>
+        <v>0.81716461063346002</v>
       </c>
       <c r="AA125" s="6">
-        <v>-1.1799545954122412</v>
+        <v>-1.1799545954122463</v>
       </c>
       <c r="AB125" s="6">
-        <v>2.4990128474560493</v>
+        <v>2.4990128474560458</v>
       </c>
       <c r="AC125" s="6">
-        <v>2.1717940267810407</v>
+        <v>2.1717940267810456</v>
       </c>
       <c r="AD125" s="6">
-        <v>7.028088547576619</v>
+        <v>7.0280885475766164</v>
       </c>
       <c r="AE125" s="6">
-        <v>-0.40313478366491046</v>
+        <v>-0.4031347836649174</v>
       </c>
       <c r="AF125" s="6">
-        <v>-1.5944161483708152</v>
+        <v>-1.5944161483708297</v>
       </c>
       <c r="AG125" s="6">
-        <v>-1.5770974064457683</v>
+        <v>-1.5770974064457877</v>
       </c>
       <c r="AH125" s="6">
-        <v>2.448701360338581</v>
+        <v>2.448701360338585</v>
       </c>
       <c r="AI125" s="6">
-        <v>1.6107182716413377</v>
+        <v>1.6107182716413229</v>
       </c>
       <c r="AJ125" s="6">
-        <v>0.96376882112283924</v>
+        <v>0.96376882112283402</v>
       </c>
       <c r="AK125" s="6">
-        <v>2.0226885337266642</v>
+        <v>2.0226885337266625</v>
       </c>
       <c r="AL125" s="6">
-        <v>-5.3804082607619749E-2</v>
+        <v>-5.3804082607641329E-2</v>
       </c>
       <c r="AM125" s="6">
-        <v>1.8242209949196813</v>
+        <v>1.8242209949196853</v>
       </c>
       <c r="AN125" s="6">
-        <v>1.4293445119353521</v>
+        <v>1.4293445119353583</v>
       </c>
       <c r="AO125" s="6">
-        <v>-8.6763757948297077E-2</v>
+        <v>-8.6763757948294176E-2</v>
       </c>
       <c r="AP125" s="6">
         <v>5.7219871604904782</v>
       </c>
       <c r="AQ125" s="6">
-        <v>1.7918511131520765</v>
+        <v>1.7918511131520856</v>
       </c>
       <c r="AR125" s="6">
-        <v>-0.95077373040645519</v>
+        <v>-0.95077373040644131</v>
       </c>
       <c r="AS125" s="6">
-        <v>-1.1764642333036401</v>
+        <v>-1.1764642333036308</v>
       </c>
       <c r="AT125" s="6">
-        <v>1.6922330774343388</v>
+        <v>1.6922330774343477</v>
       </c>
       <c r="AU125" s="6">
-        <v>2.0200884416615374</v>
+        <v>2.0200884416615343</v>
       </c>
       <c r="AV125" s="6">
-        <v>-3.5826856614368442E-2</v>
+        <v>-3.5826856614366506E-2</v>
       </c>
       <c r="AW125" s="6">
-        <v>-0.41452650335243379</v>
+        <v>-0.41452650335243563</v>
       </c>
       <c r="AX125" s="6">
-        <v>2.5536639800113012</v>
+        <v>2.5536639800113097</v>
       </c>
       <c r="AY125" s="6">
-        <v>4.0638200480830333</v>
+        <v>4.0638200480830386</v>
       </c>
       <c r="AZ125" s="6">
-        <v>3.7328225829093094</v>
+        <v>3.7328225829093147</v>
       </c>
       <c r="BA125" s="6">
-        <v>5.2393381908174277</v>
+        <v>5.2393381908174215</v>
       </c>
     </row>
     <row r="126" spans="1:53" x14ac:dyDescent="0.2">
@@ -21947,160 +21947,160 @@
         <v>43101</v>
       </c>
       <c r="B126" s="6">
-        <v>0.68470459788204752</v>
+        <v>0.68470459788206262</v>
       </c>
       <c r="C126" s="6">
-        <v>-2.326569946802636</v>
+        <v>-2.3265699468026111</v>
       </c>
       <c r="D126" s="6">
-        <v>-0.1144643726773874</v>
+        <v>-0.11446437267738366</v>
       </c>
       <c r="E126" s="6">
-        <v>1.5535583419342311</v>
+        <v>1.5535583419342325</v>
       </c>
       <c r="F126" s="6">
-        <v>1.3309851613976806</v>
+        <v>1.330985161397664</v>
       </c>
       <c r="G126" s="6">
-        <v>-1.4719917895166781</v>
+        <v>-1.471991789516645</v>
       </c>
       <c r="H126" s="6">
-        <v>1.0986789219512485</v>
+        <v>1.0986789219512452</v>
       </c>
       <c r="I126" s="6">
-        <v>-1.166367728329825</v>
+        <v>-1.1663677283298031</v>
       </c>
       <c r="J126" s="6">
-        <v>-0.31963373915311283</v>
+        <v>-0.31963373915310178</v>
       </c>
       <c r="K126" s="6">
-        <v>-3.5310765676111759</v>
+        <v>-3.5310765676111631</v>
       </c>
       <c r="L126" s="6">
-        <v>0.81115983978731698</v>
+        <v>0.8111598397873272</v>
       </c>
       <c r="M126" s="6">
-        <v>0.38016553784997514</v>
+        <v>0.38016553784997509</v>
       </c>
       <c r="N126" s="6">
-        <v>2.001812130673839</v>
+        <v>2.0018121306738457</v>
       </c>
       <c r="O126" s="6">
-        <v>-0.61347848207160216</v>
+        <v>-0.61347848207159217</v>
       </c>
       <c r="P126" s="6">
-        <v>-1.4140473845227948</v>
+        <v>-1.4140473845227879</v>
       </c>
       <c r="Q126" s="6">
-        <v>0.79257353559911325</v>
+        <v>0.79257353559910693</v>
       </c>
       <c r="R126" s="6">
-        <v>-0.77484649022314622</v>
+        <v>-0.77484649022315122</v>
       </c>
       <c r="S126" s="6">
-        <v>-1.4428493046099369</v>
+        <v>-1.4428493046099211</v>
       </c>
       <c r="T126" s="6">
-        <v>-5.0799081074885102</v>
+        <v>-5.0799081074884986</v>
       </c>
       <c r="U126" s="6">
-        <v>-2.5762625448226406</v>
+        <v>-2.5762625448226415</v>
       </c>
       <c r="V126" s="6">
-        <v>1.6311292886346795</v>
+        <v>1.631129288634696</v>
       </c>
       <c r="W126" s="6">
-        <v>0.54913242629043091</v>
+        <v>0.5491324262904379</v>
       </c>
       <c r="X126" s="6">
-        <v>-2.2002379802007619</v>
+        <v>-2.2002379802007406</v>
       </c>
       <c r="Y126" s="6">
-        <v>0.4521335992135454</v>
+        <v>0.45213359921355106</v>
       </c>
       <c r="Z126" s="6">
-        <v>-1.7229849422372272</v>
+        <v>-1.722984942237213</v>
       </c>
       <c r="AA126" s="6">
         <v>-5.6008145898808595</v>
       </c>
       <c r="AB126" s="6">
-        <v>-0.92813458104842406</v>
+        <v>-0.92813458104841362</v>
       </c>
       <c r="AC126" s="6">
-        <v>-0.57216188965276116</v>
+        <v>-0.57216188965275094</v>
       </c>
       <c r="AD126" s="6">
-        <v>0.49524347536307822</v>
+        <v>0.49524347536309282</v>
       </c>
       <c r="AE126" s="6">
-        <v>-2.8701758414093081</v>
+        <v>-2.870175841409301</v>
       </c>
       <c r="AF126" s="6">
-        <v>-4.665239586974673</v>
+        <v>-4.6652395869746641</v>
       </c>
       <c r="AG126" s="6">
-        <v>-3.1265250298804994</v>
+        <v>-3.1265250298804745</v>
       </c>
       <c r="AH126" s="6">
-        <v>0.1464078072127295</v>
+        <v>0.14640780721273</v>
       </c>
       <c r="AI126" s="6">
-        <v>-1.6133532291141826</v>
+        <v>-1.6133532291141901</v>
       </c>
       <c r="AJ126" s="6">
-        <v>0.64701371498230154</v>
+        <v>0.64701371498230609</v>
       </c>
       <c r="AK126" s="6">
-        <v>-1.4999562610096975</v>
+        <v>-1.4999562610096853</v>
       </c>
       <c r="AL126" s="6">
-        <v>-1.30375019423087</v>
+        <v>-1.3037501942308605</v>
       </c>
       <c r="AM126" s="6">
-        <v>-1.295360476565272</v>
+        <v>-1.2953604765652666</v>
       </c>
       <c r="AN126" s="6">
-        <v>-2.838058888871609</v>
+        <v>-2.8380588888715992</v>
       </c>
       <c r="AO126" s="6">
-        <v>-1.4362240201923928</v>
+        <v>-1.4362240201923888</v>
       </c>
       <c r="AP126" s="6">
-        <v>2.7890664377514103</v>
+        <v>2.7890664377514156</v>
       </c>
       <c r="AQ126" s="6">
-        <v>0.56777743914872902</v>
+        <v>0.56777743914873069</v>
       </c>
       <c r="AR126" s="6">
-        <v>-3.8597746339977701</v>
+        <v>-3.8597746339977692</v>
       </c>
       <c r="AS126" s="6">
-        <v>-5.7449079160650038</v>
+        <v>-5.7449079160650003</v>
       </c>
       <c r="AT126" s="6">
-        <v>-1.9445048884201839</v>
+        <v>-1.9445048884201899</v>
       </c>
       <c r="AU126" s="6">
-        <v>-1.6210805121045377</v>
+        <v>-1.621080512104536</v>
       </c>
       <c r="AV126" s="6">
-        <v>-1.0051055360351415</v>
+        <v>-1.0051055360351338</v>
       </c>
       <c r="AW126" s="6">
-        <v>-3.0601473655856104</v>
+        <v>-3.0601473655856153</v>
       </c>
       <c r="AX126" s="6">
-        <v>-1.5878987093989148</v>
+        <v>-1.5878987093988883</v>
       </c>
       <c r="AY126" s="6">
-        <v>2.3222346612901292</v>
+        <v>2.3222346612901288</v>
       </c>
       <c r="AZ126" s="6">
-        <v>2.4385438971089619</v>
+        <v>2.4385438971089743</v>
       </c>
       <c r="BA126" s="6">
-        <v>3.1031976699753478</v>
+        <v>3.1031976699753505</v>
       </c>
     </row>
     <row r="127" spans="1:53" x14ac:dyDescent="0.2">
@@ -22108,160 +22108,160 @@
         <v>43132</v>
       </c>
       <c r="B127" s="6">
-        <v>0.64194902224265993</v>
+        <v>0.64194902224267647</v>
       </c>
       <c r="C127" s="6">
-        <v>0.37517665730320054</v>
+        <v>0.3751766573032268</v>
       </c>
       <c r="D127" s="6">
-        <v>2.0898963250412268</v>
+        <v>2.0898963250412352</v>
       </c>
       <c r="E127" s="6">
-        <v>1.8442329554125465</v>
+        <v>1.8442329554125698</v>
       </c>
       <c r="F127" s="6">
-        <v>1.3390484791138049</v>
+        <v>1.339048479113832</v>
       </c>
       <c r="G127" s="6">
-        <v>1.522513258120413</v>
+        <v>1.5225132581204095</v>
       </c>
       <c r="H127" s="6">
-        <v>2.5621689072407148</v>
+        <v>2.5621689072407241</v>
       </c>
       <c r="I127" s="6">
-        <v>0.80553163686850582</v>
+        <v>0.80553163686849971</v>
       </c>
       <c r="J127" s="6">
-        <v>0.89808777874741175</v>
+        <v>0.89808777874743428</v>
       </c>
       <c r="K127" s="6">
-        <v>2.000714397466782</v>
+        <v>2.0007143974667927</v>
       </c>
       <c r="L127" s="6">
-        <v>2.2617870897724912</v>
+        <v>2.2617870897725103</v>
       </c>
       <c r="M127" s="6">
-        <v>3.989192907491562</v>
+        <v>3.9891929074915886</v>
       </c>
       <c r="N127" s="6">
-        <v>3.3881847994103804</v>
+        <v>3.388184799410396</v>
       </c>
       <c r="O127" s="6">
-        <v>1.1232197872097127</v>
+        <v>1.1232197872097334</v>
       </c>
       <c r="P127" s="6">
-        <v>0.55627576877837681</v>
+        <v>0.55627576877839879</v>
       </c>
       <c r="Q127" s="6">
-        <v>2.0286915420612357</v>
+        <v>2.0286915420612566</v>
       </c>
       <c r="R127" s="6">
-        <v>-1.1099109698514056</v>
+        <v>-1.1099109698513945</v>
       </c>
       <c r="S127" s="6">
-        <v>0.27326816947833815</v>
+        <v>0.27326816947834742</v>
       </c>
       <c r="T127" s="6">
-        <v>-2.1884335934646435</v>
+        <v>-2.1884335934646191</v>
       </c>
       <c r="U127" s="6">
-        <v>-0.60865627669299238</v>
+        <v>-0.60865627669298128</v>
       </c>
       <c r="V127" s="6">
-        <v>1.9623925244582281</v>
+        <v>1.9623925244582507</v>
       </c>
       <c r="W127" s="6">
-        <v>4.3957631759650004</v>
+        <v>4.3957631759650182</v>
       </c>
       <c r="X127" s="6">
-        <v>0.9606539975734647</v>
+        <v>0.9606539975734929</v>
       </c>
       <c r="Y127" s="6">
-        <v>0.54582177055558512</v>
+        <v>0.54582177055560677</v>
       </c>
       <c r="Z127" s="6">
-        <v>-1.3834493077051944</v>
+        <v>-1.3834493077051722</v>
       </c>
       <c r="AA127" s="6">
-        <v>-3.7518887851611704</v>
+        <v>-3.7518887851611451</v>
       </c>
       <c r="AB127" s="6">
-        <v>1.9230550400170101</v>
+        <v>1.9230550400170199</v>
       </c>
       <c r="AC127" s="6">
-        <v>3.2409217940446462</v>
+        <v>3.2409217940446879</v>
       </c>
       <c r="AD127" s="6">
-        <v>1.65463169158791</v>
+        <v>1.6546316915879447</v>
       </c>
       <c r="AE127" s="6">
-        <v>-0.3462682517087709</v>
+        <v>-0.34626825170874292</v>
       </c>
       <c r="AF127" s="6">
-        <v>-2.535151124513523</v>
+        <v>-2.5351511245135097</v>
       </c>
       <c r="AG127" s="6">
-        <v>1.5763435263159586</v>
+        <v>1.576343526315976</v>
       </c>
       <c r="AH127" s="6">
-        <v>1.8505606187027475</v>
+        <v>1.8505606187027637</v>
       </c>
       <c r="AI127" s="6">
-        <v>0.76321634066690514</v>
+        <v>0.76321634066692368</v>
       </c>
       <c r="AJ127" s="6">
-        <v>2.0571154502772107</v>
+        <v>2.0571154502772164</v>
       </c>
       <c r="AK127" s="6">
-        <v>1.6370057313251178</v>
+        <v>1.6370057313251294</v>
       </c>
       <c r="AL127" s="6">
-        <v>0.99950980351734708</v>
+        <v>0.9995098035173674</v>
       </c>
       <c r="AM127" s="6">
-        <v>-0.2765748889575998</v>
+        <v>-0.27657488895758681</v>
       </c>
       <c r="AN127" s="6">
-        <v>-1.4209091056375174</v>
+        <v>-1.4209091056374947</v>
       </c>
       <c r="AO127" s="6">
-        <v>0.72386273193389195</v>
+        <v>0.72386273193390371</v>
       </c>
       <c r="AP127" s="6">
-        <v>6.6321939813828914</v>
+        <v>6.6321939813829127</v>
       </c>
       <c r="AQ127" s="6">
-        <v>3.2077574260579569</v>
+        <v>3.2077574260579707</v>
       </c>
       <c r="AR127" s="6">
-        <v>-2.23823581438866</v>
+        <v>-2.2382358143886405</v>
       </c>
       <c r="AS127" s="6">
-        <v>-1.4736135925018172</v>
+        <v>-1.4736135925017899</v>
       </c>
       <c r="AT127" s="6">
-        <v>1.2687758982011685</v>
+        <v>1.2687758982011921</v>
       </c>
       <c r="AU127" s="6">
-        <v>1.3119895663834844</v>
+        <v>1.3119895663835026</v>
       </c>
       <c r="AV127" s="6">
-        <v>1.3530291044220895</v>
+        <v>1.3530291044221199</v>
       </c>
       <c r="AW127" s="6">
-        <v>-1.4204658435945803</v>
+        <v>-1.4204658435945501</v>
       </c>
       <c r="AX127" s="6">
-        <v>2.7722725788732765</v>
+        <v>2.7722725788732938</v>
       </c>
       <c r="AY127" s="6">
-        <v>3.3093763854212166</v>
+        <v>3.3093763854212197</v>
       </c>
       <c r="AZ127" s="6">
-        <v>4.5838795364800164</v>
+        <v>4.5838795364800449</v>
       </c>
       <c r="BA127" s="6">
-        <v>4.6506869261193113</v>
+        <v>4.6506869261193229</v>
       </c>
     </row>
     <row r="128" spans="1:53" x14ac:dyDescent="0.2">
@@ -22269,160 +22269,160 @@
         <v>43160</v>
       </c>
       <c r="B128" s="6">
-        <v>0.86147135130720631</v>
+        <v>0.86147135130719521</v>
       </c>
       <c r="C128" s="6">
-        <v>1.6718600691431846</v>
+        <v>1.6718600691431824</v>
       </c>
       <c r="D128" s="6">
-        <v>0.91864490134111554</v>
+        <v>0.91864490134112109</v>
       </c>
       <c r="E128" s="6">
-        <v>2.1656794998892885</v>
+        <v>2.1656794998892743</v>
       </c>
       <c r="F128" s="6">
-        <v>1.9741775218485826</v>
+        <v>1.9741775218485715</v>
       </c>
       <c r="G128" s="6">
-        <v>0.40619912844644063</v>
+        <v>0.40619912844644324</v>
       </c>
       <c r="H128" s="6">
-        <v>3.6009213040178039</v>
+        <v>3.6009213040178114</v>
       </c>
       <c r="I128" s="6">
-        <v>0.50615412107046087</v>
+        <v>0.50615412107046043</v>
       </c>
       <c r="J128" s="6">
-        <v>0.90312498600986535</v>
+        <v>0.90312498600985791</v>
       </c>
       <c r="K128" s="6">
-        <v>2.0587315202615346</v>
+        <v>2.0587315202615186</v>
       </c>
       <c r="L128" s="6">
-        <v>2.2880683787704177</v>
+        <v>2.2880683787704066</v>
       </c>
       <c r="M128" s="6">
-        <v>3.8688902221317947</v>
+        <v>3.8688902221317765</v>
       </c>
       <c r="N128" s="6">
-        <v>4.2939607418315848</v>
+        <v>4.2939607418315715</v>
       </c>
       <c r="O128" s="6">
-        <v>0.60138084469872699</v>
+        <v>0.60138084469872388</v>
       </c>
       <c r="P128" s="6">
-        <v>1.1198188728869054</v>
+        <v>1.1198188728869027</v>
       </c>
       <c r="Q128" s="6">
-        <v>3.6383443798160324</v>
+        <v>3.6383443798160289</v>
       </c>
       <c r="R128" s="6">
-        <v>-0.26083552255222808</v>
+        <v>-0.26083552255223463</v>
       </c>
       <c r="S128" s="6">
-        <v>0.39352541429166404</v>
+        <v>0.39352541429166865</v>
       </c>
       <c r="T128" s="6">
-        <v>-2.0356766309326328</v>
+        <v>-2.0356766309326249</v>
       </c>
       <c r="U128" s="6">
-        <v>0.7279981739449688</v>
+        <v>0.72799817394496369</v>
       </c>
       <c r="V128" s="6">
-        <v>-1.4915830899232925</v>
+        <v>-1.4915830899232838</v>
       </c>
       <c r="W128" s="6">
         <v>4.6182171139336692</v>
       </c>
       <c r="X128" s="6">
-        <v>-0.52352069922801614</v>
+        <v>-0.52352069922803279</v>
       </c>
       <c r="Y128" s="6">
-        <v>1.0207453021699266</v>
+        <v>1.0207453021699131</v>
       </c>
       <c r="Z128" s="6">
-        <v>-0.52692718265478078</v>
+        <v>-0.52692718265478045</v>
       </c>
       <c r="AA128" s="6">
-        <v>-2.7491510481305994</v>
+        <v>-2.7491510481305999</v>
       </c>
       <c r="AB128" s="6">
-        <v>1.033720382540384</v>
+        <v>1.033720382540374</v>
       </c>
       <c r="AC128" s="6">
-        <v>3.6704178091397277</v>
+        <v>3.6704178091397255</v>
       </c>
       <c r="AD128" s="6">
-        <v>0.29966848057968404</v>
+        <v>0.29966848057968781</v>
       </c>
       <c r="AE128" s="6">
-        <v>-0.4353738003180862</v>
+        <v>-0.4353738003180907</v>
       </c>
       <c r="AF128" s="6">
-        <v>-4.9461232192300288</v>
+        <v>-4.9461232192300333</v>
       </c>
       <c r="AG128" s="6">
-        <v>2.8220281935724687</v>
+        <v>2.8220281935724598</v>
       </c>
       <c r="AH128" s="6">
-        <v>1.8982284845307704</v>
+        <v>1.8982284845307513</v>
       </c>
       <c r="AI128" s="6">
-        <v>0.93339924139996289</v>
+        <v>0.93339924139996755</v>
       </c>
       <c r="AJ128" s="6">
-        <v>1.4978926012817761</v>
+        <v>1.4978926012817682</v>
       </c>
       <c r="AK128" s="6">
-        <v>1.7208898807869724</v>
+        <v>1.7208898807869688</v>
       </c>
       <c r="AL128" s="6">
-        <v>1.0209533985736754</v>
+        <v>1.0209533985736694</v>
       </c>
       <c r="AM128" s="6">
-        <v>-0.90380409448114229</v>
+        <v>-0.90380409448112242</v>
       </c>
       <c r="AN128" s="6">
-        <v>-1.3344479198822432</v>
+        <v>-1.334447919882237</v>
       </c>
       <c r="AO128" s="6">
-        <v>1.2904133754760441</v>
+        <v>1.2904133754760521</v>
       </c>
       <c r="AP128" s="6">
-        <v>3.8108539298786508</v>
+        <v>3.8108539298786437</v>
       </c>
       <c r="AQ128" s="6">
-        <v>1.4058214501880799</v>
+        <v>1.4058214501880575</v>
       </c>
       <c r="AR128" s="6">
-        <v>-2.5702050078366225</v>
+        <v>-2.5702050078366292</v>
       </c>
       <c r="AS128" s="6">
-        <v>-0.14369050291848043</v>
+        <v>-0.14369050291849025</v>
       </c>
       <c r="AT128" s="6">
-        <v>1.0031778993895599</v>
+        <v>1.0031778993895573</v>
       </c>
       <c r="AU128" s="6">
-        <v>0.92454833685242077</v>
+        <v>0.92454833685242521</v>
       </c>
       <c r="AV128" s="6">
-        <v>1.741490929198634</v>
+        <v>1.7414909291986282</v>
       </c>
       <c r="AW128" s="6">
-        <v>-0.23572526211291617</v>
+        <v>-0.23572526211292169</v>
       </c>
       <c r="AX128" s="6">
-        <v>1.9968471007602677</v>
+        <v>1.9968471007602648</v>
       </c>
       <c r="AY128" s="6">
-        <v>1.9269154278840104</v>
+        <v>1.9269154278840059</v>
       </c>
       <c r="AZ128" s="6">
-        <v>3.467636854330125</v>
+        <v>3.4676368543301312</v>
       </c>
       <c r="BA128" s="6">
-        <v>6.5284148681722183</v>
+        <v>6.5284148681722067</v>
       </c>
     </row>
     <row r="129" spans="1:53" x14ac:dyDescent="0.2">
@@ -22430,160 +22430,160 @@
         <v>43191</v>
       </c>
       <c r="B129" s="6">
-        <v>0.4606517338917126</v>
+        <v>0.4606517338917297</v>
       </c>
       <c r="C129" s="6">
-        <v>0.76516524274620978</v>
+        <v>0.76516524274621567</v>
       </c>
       <c r="D129" s="6">
-        <v>-0.73299770171497336</v>
+        <v>-0.73299770171495726</v>
       </c>
       <c r="E129" s="6">
-        <v>-7.6513938688543365E-2</v>
+        <v>-7.6513938688533845E-2</v>
       </c>
       <c r="F129" s="6">
-        <v>0.81882002715023294</v>
+        <v>0.81882002715024238</v>
       </c>
       <c r="G129" s="6">
-        <v>0.76962531304973081</v>
+        <v>0.76962531304975257</v>
       </c>
       <c r="H129" s="6">
-        <v>1.928499348434255</v>
+        <v>1.9284993484342701</v>
       </c>
       <c r="I129" s="6">
-        <v>0.32859691471343727</v>
+        <v>0.32859691471344954</v>
       </c>
       <c r="J129" s="6">
-        <v>-1.7696160045674751</v>
+        <v>-1.769616004567456</v>
       </c>
       <c r="K129" s="6">
-        <v>3.6005054957085543</v>
+        <v>3.6005054957085685</v>
       </c>
       <c r="L129" s="6">
-        <v>1.7573524377525529</v>
+        <v>1.7573524377525747</v>
       </c>
       <c r="M129" s="6">
-        <v>3.426932152109071</v>
+        <v>3.4269321521090856</v>
       </c>
       <c r="N129" s="6">
-        <v>3.7059861919792674</v>
+        <v>3.7059861919792749</v>
       </c>
       <c r="O129" s="6">
-        <v>0.41163342672401998</v>
+        <v>0.4116334267240454</v>
       </c>
       <c r="P129" s="6">
-        <v>1.5663518774600804</v>
+        <v>1.5663518774600846</v>
       </c>
       <c r="Q129" s="6">
-        <v>1.6566192886707094</v>
+        <v>1.6566192886707087</v>
       </c>
       <c r="R129" s="6">
-        <v>-1.5177961054014615</v>
+        <v>-1.5177961054014359</v>
       </c>
       <c r="S129" s="6">
-        <v>1.7489672722223557</v>
+        <v>1.7489672722223588</v>
       </c>
       <c r="T129" s="6">
-        <v>-1.2791236756732254</v>
+        <v>-1.2791236756732169</v>
       </c>
       <c r="U129" s="6">
-        <v>2.592764017634646</v>
+        <v>2.592764017634654</v>
       </c>
       <c r="V129" s="6">
-        <v>1.2117273648978617</v>
+        <v>1.2117273648978781</v>
       </c>
       <c r="W129" s="6">
-        <v>5.8841174876214941</v>
+        <v>5.8841174876215065</v>
       </c>
       <c r="X129" s="6">
-        <v>0.77008359542527405</v>
+        <v>0.77008359542527649</v>
       </c>
       <c r="Y129" s="6">
-        <v>0.87645769993820399</v>
+        <v>0.87645769993821265</v>
       </c>
       <c r="Z129" s="6">
-        <v>-2.4707426931389143</v>
+        <v>-2.4707426931389018</v>
       </c>
       <c r="AA129" s="6">
-        <v>-2.5170509835989368</v>
+        <v>-2.5170509835989119</v>
       </c>
       <c r="AB129" s="6">
-        <v>0.7550620228504541</v>
+        <v>0.75506202285045532</v>
       </c>
       <c r="AC129" s="6">
-        <v>1.7222841672692346</v>
+        <v>1.7222841672692515</v>
       </c>
       <c r="AD129" s="6">
-        <v>0.52883429895568579</v>
+        <v>0.52883429895570111</v>
       </c>
       <c r="AE129" s="6">
-        <v>0.35197383059046639</v>
+        <v>0.35197383059048953</v>
       </c>
       <c r="AF129" s="6">
-        <v>-4.4571257447080832</v>
+        <v>-4.4571257447080557</v>
       </c>
       <c r="AG129" s="6">
-        <v>1.0468188966580085</v>
+        <v>1.0468188966580274</v>
       </c>
       <c r="AH129" s="6">
-        <v>0.7123965450877503</v>
+        <v>0.71239654508777239</v>
       </c>
       <c r="AI129" s="6">
-        <v>0.13094756158210488</v>
+        <v>0.13094756158212287</v>
       </c>
       <c r="AJ129" s="6">
-        <v>1.892195943910437</v>
+        <v>1.8921959439104619</v>
       </c>
       <c r="AK129" s="6">
-        <v>-0.97880840145314996</v>
+        <v>-0.97880840145313808</v>
       </c>
       <c r="AL129" s="6">
-        <v>1.5261895743910394</v>
+        <v>1.5261895743910598</v>
       </c>
       <c r="AM129" s="6">
-        <v>-1.3397448256555076</v>
+        <v>-1.3397448256554949</v>
       </c>
       <c r="AN129" s="6">
-        <v>-1.4492248085337798</v>
+        <v>-1.4492248085337718</v>
       </c>
       <c r="AO129" s="6">
-        <v>0.70731618507029048</v>
+        <v>0.70731618507030203</v>
       </c>
       <c r="AP129" s="6">
-        <v>2.9893502361458526</v>
+        <v>2.9893502361458708</v>
       </c>
       <c r="AQ129" s="6">
-        <v>3.5781115079097701</v>
+        <v>3.5781115079097798</v>
       </c>
       <c r="AR129" s="6">
-        <v>-1.79779844701765</v>
+        <v>-1.79779844701763</v>
       </c>
       <c r="AS129" s="6">
-        <v>0.54807707374501935</v>
+        <v>0.54807707374502801</v>
       </c>
       <c r="AT129" s="6">
-        <v>0.99446998930807196</v>
+        <v>0.99446998930808506</v>
       </c>
       <c r="AU129" s="6">
-        <v>0.34796265958696732</v>
+        <v>0.34796265958698958</v>
       </c>
       <c r="AV129" s="6">
-        <v>0.7703176263041549</v>
+        <v>0.770317626304169</v>
       </c>
       <c r="AW129" s="6">
-        <v>-0.3632381663233693</v>
+        <v>-0.36323816632335987</v>
       </c>
       <c r="AX129" s="6">
-        <v>1.7021229031375176</v>
+        <v>1.7021229031375225</v>
       </c>
       <c r="AY129" s="6">
-        <v>4.3978552846743462</v>
+        <v>4.397855284674355</v>
       </c>
       <c r="AZ129" s="6">
-        <v>2.4293432193194415</v>
+        <v>2.4293432193194402</v>
       </c>
       <c r="BA129" s="6">
-        <v>2.8877878464510425</v>
+        <v>2.8877878464510598</v>
       </c>
     </row>
     <row r="130" spans="1:53" x14ac:dyDescent="0.2">
@@ -22591,160 +22591,160 @@
         <v>43221</v>
       </c>
       <c r="B130" s="6">
-        <v>0.27571351105983699</v>
+        <v>0.27571351105983999</v>
       </c>
       <c r="C130" s="6">
-        <v>5.5526770840742907E-3</v>
+        <v>5.5526770840747522E-3</v>
       </c>
       <c r="D130" s="6">
-        <v>-2.1798963503787587</v>
+        <v>-2.1798963503787632</v>
       </c>
       <c r="E130" s="6">
-        <v>0.4366137552239186</v>
+        <v>0.43661375522392004</v>
       </c>
       <c r="F130" s="6">
-        <v>-0.34612516142080541</v>
+        <v>-0.34612516142079242</v>
       </c>
       <c r="G130" s="6">
-        <v>8.5563344556126408E-2</v>
+        <v>8.5563344556111615E-2</v>
       </c>
       <c r="H130" s="6">
-        <v>2.4124047695187856</v>
+        <v>2.4124047695187847</v>
       </c>
       <c r="I130" s="6">
-        <v>-0.71781399648653954</v>
+        <v>-0.7178139964865381</v>
       </c>
       <c r="J130" s="6">
-        <v>0.58175812239612168</v>
+        <v>0.58175812239611813</v>
       </c>
       <c r="K130" s="6">
-        <v>2.4484852418811731</v>
+        <v>2.4484852418811598</v>
       </c>
       <c r="L130" s="6">
-        <v>2.3330460157556363</v>
+        <v>2.333046015755647</v>
       </c>
       <c r="M130" s="6">
-        <v>2.7630749620399131</v>
+        <v>2.7630749620399149</v>
       </c>
       <c r="N130" s="6">
-        <v>2.1406836625691348</v>
+        <v>2.1406836625691414</v>
       </c>
       <c r="O130" s="6">
-        <v>0.31107461234613865</v>
+        <v>0.31107461234614059</v>
       </c>
       <c r="P130" s="6">
-        <v>0.61526909701839749</v>
+        <v>0.61526909701838695</v>
       </c>
       <c r="Q130" s="6">
-        <v>-1.1254331779805027</v>
+        <v>-1.1254331779805034</v>
       </c>
       <c r="R130" s="6">
-        <v>1.2310089222314045</v>
+        <v>1.2310089222313965</v>
       </c>
       <c r="S130" s="6">
-        <v>1.4616555809999776</v>
+        <v>1.461655580999986</v>
       </c>
       <c r="T130" s="6">
-        <v>-1.4468857554096688</v>
+        <v>-1.4468857554096703</v>
       </c>
       <c r="U130" s="6">
-        <v>1.3308554802288544</v>
+        <v>1.3308554802288515</v>
       </c>
       <c r="V130" s="6">
-        <v>-0.39088174920787688</v>
+        <v>-0.39088174920786556</v>
       </c>
       <c r="W130" s="6">
-        <v>4.8297862810473147</v>
+        <v>4.8297862810473156</v>
       </c>
       <c r="X130" s="6">
-        <v>1.2329631947018465</v>
+        <v>1.2329631947018482</v>
       </c>
       <c r="Y130" s="6">
-        <v>1.1898296316681929</v>
+        <v>1.1898296316681842</v>
       </c>
       <c r="Z130" s="6">
-        <v>-0.26254104365955977</v>
+        <v>-0.26254104365956593</v>
       </c>
       <c r="AA130" s="6">
-        <v>-3.1794452173334058</v>
+        <v>-3.1794452173334133</v>
       </c>
       <c r="AB130" s="6">
-        <v>1.4441612517794529</v>
+        <v>1.4441612517794422</v>
       </c>
       <c r="AC130" s="6">
-        <v>2.6846015618401902</v>
+        <v>2.68460156184018</v>
       </c>
       <c r="AD130" s="6">
-        <v>-0.74302353682429056</v>
+        <v>-0.74302353682428557</v>
       </c>
       <c r="AE130" s="6">
-        <v>1.0401024477925582</v>
+        <v>1.0401024477925584</v>
       </c>
       <c r="AF130" s="6">
-        <v>-3.3523739769426784</v>
+        <v>-3.3523739769426566</v>
       </c>
       <c r="AG130" s="6">
-        <v>-3.4032723836531256</v>
+        <v>-3.4032723836531158</v>
       </c>
       <c r="AH130" s="6">
-        <v>0.8231721284329937</v>
+        <v>0.82317212843298204</v>
       </c>
       <c r="AI130" s="6">
-        <v>0.11108451236694056</v>
+        <v>0.11108451236693005</v>
       </c>
       <c r="AJ130" s="6">
-        <v>1.5252279345312769</v>
+        <v>1.5252279345312898</v>
       </c>
       <c r="AK130" s="6">
-        <v>-0.82091184953997298</v>
+        <v>-0.82091184953997032</v>
       </c>
       <c r="AL130" s="6">
-        <v>0.18295087982000055</v>
+        <v>0.18295087981998881</v>
       </c>
       <c r="AM130" s="6">
-        <v>-0.92854178514681363</v>
+        <v>-0.92854178514680374</v>
       </c>
       <c r="AN130" s="6">
-        <v>0.53048861452856155</v>
+        <v>0.53048861452856788</v>
       </c>
       <c r="AO130" s="6">
-        <v>1.0218768309241142</v>
+        <v>1.0218768309241177</v>
       </c>
       <c r="AP130" s="6">
-        <v>2.8025019577232171</v>
+        <v>2.802501957723218</v>
       </c>
       <c r="AQ130" s="6">
-        <v>2.3043261208103254</v>
+        <v>2.3043261208103361</v>
       </c>
       <c r="AR130" s="6">
-        <v>-1.1978444729056565</v>
+        <v>-1.1978444729056557</v>
       </c>
       <c r="AS130" s="6">
-        <v>-0.12143506777405669</v>
+        <v>-0.12143506777405028</v>
       </c>
       <c r="AT130" s="6">
-        <v>-0.38412678606462458</v>
+        <v>-0.38412678606463069</v>
       </c>
       <c r="AU130" s="6">
-        <v>0.59648881648315144</v>
+        <v>0.59648881648315766</v>
       </c>
       <c r="AV130" s="6">
-        <v>0.16446143959695556</v>
+        <v>0.16446143959694737</v>
       </c>
       <c r="AW130" s="6">
-        <v>0.27711345739873133</v>
+        <v>0.27711345739873289</v>
       </c>
       <c r="AX130" s="6">
-        <v>1.5900550205616955</v>
+        <v>1.5900550205616801</v>
       </c>
       <c r="AY130" s="6">
-        <v>3.0003369087140808</v>
+        <v>3.0003369087140745</v>
       </c>
       <c r="AZ130" s="6">
-        <v>3.4148143451810524</v>
+        <v>3.4148143451810622</v>
       </c>
       <c r="BA130" s="6">
-        <v>2.8169369070762382</v>
+        <v>2.8169369070762338</v>
       </c>
     </row>
     <row r="131" spans="1:53" x14ac:dyDescent="0.2">
@@ -22752,160 +22752,160 @@
         <v>43252</v>
       </c>
       <c r="B131" s="6">
-        <v>0.4917958602642416</v>
+        <v>0.49179586026423172</v>
       </c>
       <c r="C131" s="6">
-        <v>1.2164817963925705</v>
+        <v>1.2164817963925738</v>
       </c>
       <c r="D131" s="6">
-        <v>-1.7293571821812341</v>
+        <v>-1.7293571821812275</v>
       </c>
       <c r="E131" s="6">
-        <v>0.61280082125751478</v>
+        <v>0.6128008212575129</v>
       </c>
       <c r="F131" s="6">
-        <v>-4.1503706275721981E-2</v>
+        <v>-4.1503706275711309E-2</v>
       </c>
       <c r="G131" s="6">
-        <v>0.37955269592626151</v>
+        <v>0.37955269592626817</v>
       </c>
       <c r="H131" s="6">
-        <v>2.5057149310100342</v>
+        <v>2.5057149310100324</v>
       </c>
       <c r="I131" s="6">
-        <v>-0.21128097697562928</v>
+        <v>-0.21128097697563208</v>
       </c>
       <c r="J131" s="6">
-        <v>-8.4108458365665388</v>
+        <v>-8.4108458365665211</v>
       </c>
       <c r="K131" s="6">
-        <v>3.5958304909862044</v>
+        <v>3.5958304909862253</v>
       </c>
       <c r="L131" s="6">
-        <v>3.6048781350570778</v>
+        <v>3.6048781350570809</v>
       </c>
       <c r="M131" s="6">
-        <v>-1.004496460088915</v>
+        <v>-1.0044964600889064</v>
       </c>
       <c r="N131" s="6">
-        <v>2.9869627658870157</v>
+        <v>2.9869627658870184</v>
       </c>
       <c r="O131" s="6">
-        <v>0.73674294486528313</v>
+        <v>0.73674294486528868</v>
       </c>
       <c r="P131" s="6">
-        <v>0.25382398530819195</v>
+        <v>0.25382398530820399</v>
       </c>
       <c r="Q131" s="6">
-        <v>-2.6068659612836749</v>
+        <v>-2.6068659612836655</v>
       </c>
       <c r="R131" s="6">
-        <v>1.2990212392169551</v>
+        <v>1.2990212392169704</v>
       </c>
       <c r="S131" s="6">
-        <v>2.6110865501644507</v>
+        <v>2.6110865501644493</v>
       </c>
       <c r="T131" s="6">
-        <v>-2.0194687903511968</v>
+        <v>-2.0194687903511865</v>
       </c>
       <c r="U131" s="6">
-        <v>2.0870060409441908</v>
+        <v>2.0870060409441993</v>
       </c>
       <c r="V131" s="6">
-        <v>0.94615008900095354</v>
+        <v>0.94615008900095088</v>
       </c>
       <c r="W131" s="6">
-        <v>2.6234413449563099</v>
+        <v>2.6234413449563139</v>
       </c>
       <c r="X131" s="6">
-        <v>1.4774967194657129</v>
+        <v>1.4774967194657147</v>
       </c>
       <c r="Y131" s="6">
-        <v>1.9573245725943518</v>
+        <v>1.9573245725943544</v>
       </c>
       <c r="Z131" s="6">
-        <v>9.706352226003348E-2</v>
+        <v>9.7063522260029178E-2</v>
       </c>
       <c r="AA131" s="6">
-        <v>-3.1174559812270313</v>
+        <v>-3.1174559812270251</v>
       </c>
       <c r="AB131" s="6">
-        <v>0.82164558218181705</v>
+        <v>0.82164558218182115</v>
       </c>
       <c r="AC131" s="6">
-        <v>2.4412795113149066</v>
+        <v>2.4412795113149235</v>
       </c>
       <c r="AD131" s="6">
-        <v>-0.64258863756359197</v>
+        <v>-0.64258863756359408</v>
       </c>
       <c r="AE131" s="6">
-        <v>0.91778199035619812</v>
+        <v>0.91778199035619856</v>
       </c>
       <c r="AF131" s="6">
-        <v>-3.5330377457006503</v>
+        <v>-3.5330377457006392</v>
       </c>
       <c r="AG131" s="6">
-        <v>-2.9343109741014293</v>
+        <v>-2.9343109741014333</v>
       </c>
       <c r="AH131" s="6">
-        <v>8.2761654307312221E-2</v>
+        <v>8.2761654307329915E-2</v>
       </c>
       <c r="AI131" s="6">
-        <v>-0.24208139662574329</v>
+        <v>-0.24208139662574574</v>
       </c>
       <c r="AJ131" s="6">
-        <v>1.3075819029912272</v>
+        <v>1.3075819029912374</v>
       </c>
       <c r="AK131" s="6">
-        <v>0.39980532727215856</v>
+        <v>0.39980532727215751</v>
       </c>
       <c r="AL131" s="6">
-        <v>-4.3061762310728773E-2</v>
+        <v>-4.3061762310738924E-2</v>
       </c>
       <c r="AM131" s="6">
-        <v>0.71127254449182975</v>
+        <v>0.71127254449184141</v>
       </c>
       <c r="AN131" s="6">
-        <v>-6.3403075016594562E-2</v>
+        <v>-6.3403075016581031E-2</v>
       </c>
       <c r="AO131" s="6">
-        <v>0.67267899142321597</v>
+        <v>0.67267899142322896</v>
       </c>
       <c r="AP131" s="6">
-        <v>1.7404443639100404</v>
+        <v>1.7404443639100626</v>
       </c>
       <c r="AQ131" s="6">
-        <v>1.0018243473343866</v>
+        <v>1.0018243473343913</v>
       </c>
       <c r="AR131" s="6">
-        <v>0.81958507253039792</v>
+        <v>0.81958507253041235</v>
       </c>
       <c r="AS131" s="6">
-        <v>1.0582969329341503</v>
+        <v>1.0582969329341472</v>
       </c>
       <c r="AT131" s="6">
-        <v>0.21693973549814213</v>
+        <v>0.21693973549814421</v>
       </c>
       <c r="AU131" s="6">
-        <v>-0.45370972431114004</v>
+        <v>-0.45370972431113638</v>
       </c>
       <c r="AV131" s="6">
-        <v>1.314611615909886</v>
+        <v>1.3146116159098828</v>
       </c>
       <c r="AW131" s="6">
-        <v>1.2436235717176254</v>
+        <v>1.2436235717176221</v>
       </c>
       <c r="AX131" s="6">
-        <v>2.12567293774095</v>
+        <v>2.1256729377409691</v>
       </c>
       <c r="AY131" s="6">
-        <v>1.6608530842487459</v>
+        <v>1.6608530842487528</v>
       </c>
       <c r="AZ131" s="6">
-        <v>3.12613039079134</v>
+        <v>3.1261303907913507</v>
       </c>
       <c r="BA131" s="6">
-        <v>4.5008415480829189</v>
+        <v>4.5008415480829118</v>
       </c>
     </row>
     <row r="132" spans="1:53" x14ac:dyDescent="0.2">
@@ -22913,160 +22913,160 @@
         <v>43282</v>
       </c>
       <c r="B132" s="6">
-        <v>0.11732566637096427</v>
+        <v>0.11732566637094996</v>
       </c>
       <c r="C132" s="6">
-        <v>0.77776378128132473</v>
+        <v>0.77776378128130119</v>
       </c>
       <c r="D132" s="6">
-        <v>-0.82287226087625243</v>
+        <v>-0.82287226087627929</v>
       </c>
       <c r="E132" s="6">
-        <v>-1.6806095961238325</v>
+        <v>-1.6806095961238419</v>
       </c>
       <c r="F132" s="6">
-        <v>0.24341595772349839</v>
+        <v>0.24341595772349192</v>
       </c>
       <c r="G132" s="6">
-        <v>-0.66124730031487622</v>
+        <v>-0.6612473003148841</v>
       </c>
       <c r="H132" s="6">
-        <v>1.3987273414620414</v>
+        <v>1.3987273414620285</v>
       </c>
       <c r="I132" s="6">
-        <v>0.74801474426288428</v>
+        <v>0.74801474426289649</v>
       </c>
       <c r="J132" s="6">
-        <v>-6.1446124506191113</v>
+        <v>-6.1446124506191291</v>
       </c>
       <c r="K132" s="6">
-        <v>1.7229125772525828</v>
+        <v>1.7229125772525709</v>
       </c>
       <c r="L132" s="6">
-        <v>1.6105057329342982</v>
+        <v>1.610505732934294</v>
       </c>
       <c r="M132" s="6">
-        <v>-1.4578983048513117</v>
+        <v>-1.4578983048513305</v>
       </c>
       <c r="N132" s="6">
         <v>2.0843347501665903</v>
       </c>
       <c r="O132" s="6">
-        <v>1.1389294471699792E-2</v>
+        <v>1.1389294471683985E-2</v>
       </c>
       <c r="P132" s="6">
-        <v>1.333110779560291</v>
+        <v>1.3331107795602846</v>
       </c>
       <c r="Q132" s="6">
-        <v>-2.4296992225268177</v>
+        <v>-2.429699222526839</v>
       </c>
       <c r="R132" s="6">
-        <v>1.0357996065648853</v>
+        <v>1.0357996065648831</v>
       </c>
       <c r="S132" s="6">
-        <v>2.1654403897082961</v>
+        <v>2.1654403897082837</v>
       </c>
       <c r="T132" s="6">
-        <v>-2.067342354584254</v>
+        <v>-2.0673423545842633</v>
       </c>
       <c r="U132" s="6">
-        <v>0.51744248159981632</v>
+        <v>0.51744248159979622</v>
       </c>
       <c r="V132" s="6">
-        <v>0.47917715179836934</v>
+        <v>0.47917715179837006</v>
       </c>
       <c r="W132" s="6">
-        <v>2.3298974357705395</v>
+        <v>2.3298974357705311</v>
       </c>
       <c r="X132" s="6">
-        <v>0.51626152611230292</v>
+        <v>0.51626152611228138</v>
       </c>
       <c r="Y132" s="6">
-        <v>1.4283109429416461</v>
+        <v>1.4283109429416507</v>
       </c>
       <c r="Z132" s="6">
-        <v>-0.89876409960907155</v>
+        <v>-0.89876409960908088</v>
       </c>
       <c r="AA132" s="6">
-        <v>-3.6995966977381509</v>
+        <v>-3.69959669773817</v>
       </c>
       <c r="AB132" s="6">
-        <v>1.1801058950052254</v>
+        <v>1.1801058950052106</v>
       </c>
       <c r="AC132" s="6">
-        <v>1.4441172798326285</v>
+        <v>1.4441172798326061</v>
       </c>
       <c r="AD132" s="6">
-        <v>-1.1140450681415714</v>
+        <v>-1.1140450681415888</v>
       </c>
       <c r="AE132" s="6">
-        <v>0.5271315382065821</v>
+        <v>0.52713153820656422</v>
       </c>
       <c r="AF132" s="6">
-        <v>-2.1791379272859843</v>
+        <v>-2.1791379272859981</v>
       </c>
       <c r="AG132" s="6">
-        <v>-1.6182976657245087</v>
+        <v>-1.6182976657245298</v>
       </c>
       <c r="AH132" s="6">
-        <v>0.14697830524903602</v>
+        <v>0.14697830524902306</v>
       </c>
       <c r="AI132" s="6">
-        <v>-4.1774484657886524E-2</v>
+        <v>-4.177448465791362E-2</v>
       </c>
       <c r="AJ132" s="6">
-        <v>0.11399630805167102</v>
+        <v>0.11399630805165116</v>
       </c>
       <c r="AK132" s="6">
-        <v>0.10687284641051062</v>
+        <v>0.10687284641050532</v>
       </c>
       <c r="AL132" s="6">
-        <v>-0.1265454615712317</v>
+        <v>-0.12654546157124152</v>
       </c>
       <c r="AM132" s="6">
-        <v>-0.77221893158650845</v>
+        <v>-0.772218931586518</v>
       </c>
       <c r="AN132" s="6">
-        <v>-0.1281970408948451</v>
+        <v>-0.12819704089485554</v>
       </c>
       <c r="AO132" s="6">
-        <v>1.3660094714575881</v>
+        <v>1.366009471457585</v>
       </c>
       <c r="AP132" s="6">
-        <v>1.0308476747470017</v>
+        <v>1.0308476747469906</v>
       </c>
       <c r="AQ132" s="6">
-        <v>0.99168288330019649</v>
+        <v>0.99168288330019161</v>
       </c>
       <c r="AR132" s="6">
-        <v>2.3636656655672095</v>
+        <v>2.3636656655672041</v>
       </c>
       <c r="AS132" s="6">
-        <v>0.52249582665518246</v>
+        <v>0.52249582665517336</v>
       </c>
       <c r="AT132" s="6">
-        <v>-0.25930823532336894</v>
+        <v>-0.25930823532337871</v>
       </c>
       <c r="AU132" s="6">
-        <v>-0.77458814802876241</v>
+        <v>-0.7745881480287754</v>
       </c>
       <c r="AV132" s="6">
-        <v>0.55052044057658256</v>
+        <v>0.55052044057657457</v>
       </c>
       <c r="AW132" s="6">
-        <v>0.70504986918796275</v>
+        <v>0.70504986918796186</v>
       </c>
       <c r="AX132" s="6">
-        <v>0.49939418329228724</v>
+        <v>0.49939418329228791</v>
       </c>
       <c r="AY132" s="6">
-        <v>1.6054652670412002</v>
+        <v>1.6054652670411844</v>
       </c>
       <c r="AZ132" s="6">
-        <v>2.04424650770031</v>
+        <v>2.044246507700294</v>
       </c>
       <c r="BA132" s="6">
-        <v>3.6105767207254647</v>
+        <v>3.6105767207254678</v>
       </c>
     </row>
     <row r="133" spans="1:53" x14ac:dyDescent="0.2">
@@ -23074,160 +23074,160 @@
         <v>43313</v>
       </c>
       <c r="B133" s="6">
-        <v>0.50372024160434392</v>
+        <v>0.54126085128670653</v>
       </c>
       <c r="C133" s="6">
-        <v>0.82189777027112521</v>
+        <v>0.82189777027111577</v>
       </c>
       <c r="D133" s="6">
-        <v>-1.6514161354383536</v>
+        <v>-1.6514161354383445</v>
       </c>
       <c r="E133" s="6">
-        <v>-2.0422627486964209</v>
+        <v>-2.0422627486964235</v>
       </c>
       <c r="F133" s="6">
-        <v>0.21049270419392524</v>
+        <v>0.21049270419390664</v>
       </c>
       <c r="G133" s="6">
-        <v>-0.11174211578931134</v>
+        <v>-0.11174211578931773</v>
       </c>
       <c r="H133" s="6">
-        <v>2.4777066096882328</v>
+        <v>2.4777066096882305</v>
       </c>
       <c r="I133" s="6">
-        <v>0.76479820227430673</v>
+        <v>0.7647982022743125</v>
       </c>
       <c r="J133" s="6">
-        <v>-4.4014778345361893</v>
+        <v>-4.4014778345362</v>
       </c>
       <c r="K133" s="6">
-        <v>1.9721042416692456</v>
+        <v>1.9721042416692374</v>
       </c>
       <c r="L133" s="6">
-        <v>1.9288395391008701</v>
+        <v>1.9288395391008679</v>
       </c>
       <c r="M133" s="6">
-        <v>-1.3960237514773155</v>
+        <v>-1.3960237514773239</v>
       </c>
       <c r="N133" s="6">
-        <v>1.9338196269362098</v>
+        <v>1.9338196269362093</v>
       </c>
       <c r="O133" s="6">
-        <v>-0.25494700313924118</v>
+        <v>-0.25494700313924834</v>
       </c>
       <c r="P133" s="6">
-        <v>0.81083625625520905</v>
+        <v>0.81083625625519395</v>
       </c>
       <c r="Q133" s="6">
-        <v>-1.82343927063304</v>
+        <v>-1.8234392706330598</v>
       </c>
       <c r="R133" s="6">
-        <v>1.5646282318956306</v>
+        <v>1.5646282318956337</v>
       </c>
       <c r="S133" s="6">
-        <v>1.5845949233045715</v>
+        <v>1.5845949233045591</v>
       </c>
       <c r="T133" s="6">
-        <v>-2.5559164723068983</v>
+        <v>-2.5559164723069001</v>
       </c>
       <c r="U133" s="6">
-        <v>1.4280137058005262</v>
+        <v>1.4280137058005085</v>
       </c>
       <c r="V133" s="6">
-        <v>0.14346642577328633</v>
+        <v>0.14346642577328092</v>
       </c>
       <c r="W133" s="6">
-        <v>2.201221507477253</v>
+        <v>2.2012215074772401</v>
       </c>
       <c r="X133" s="6">
-        <v>1.2337288923412575</v>
+        <v>1.2337288923412519</v>
       </c>
       <c r="Y133" s="6">
         <v>1.6562885572917982</v>
       </c>
       <c r="Z133" s="6">
-        <v>1.0906659265829061E-2</v>
+        <v>1.090665926582275E-2</v>
       </c>
       <c r="AA133" s="6">
-        <v>-4.7919346053378415</v>
+        <v>-4.7919346053378424</v>
       </c>
       <c r="AB133" s="6">
-        <v>1.3680138317200139</v>
+        <v>1.3680138317200232</v>
       </c>
       <c r="AC133" s="6">
-        <v>2.1088410808057478</v>
+        <v>2.1088410808057394</v>
       </c>
       <c r="AD133" s="6">
-        <v>-1.9803542292556549</v>
+        <v>-1.9803542292556642</v>
       </c>
       <c r="AE133" s="6">
-        <v>1.8659391270915211</v>
+        <v>1.8659391270915364</v>
       </c>
       <c r="AF133" s="6">
-        <v>-3.287861488909166</v>
+        <v>-3.2878614889091726</v>
       </c>
       <c r="AG133" s="6">
-        <v>-1.2933928750482973</v>
+        <v>-1.2933928750482917</v>
       </c>
       <c r="AH133" s="6">
-        <v>1.4297126477488404</v>
+        <v>1.4297126477488455</v>
       </c>
       <c r="AI133" s="6">
-        <v>0.70674507982937518</v>
+        <v>0.70674507982937496</v>
       </c>
       <c r="AJ133" s="6">
-        <v>1.6264687643210736</v>
+        <v>1.6264687643210547</v>
       </c>
       <c r="AK133" s="6">
-        <v>0.38735768720013708</v>
+        <v>0.38735768720013242</v>
       </c>
       <c r="AL133" s="6">
-        <v>0.70744976383170566</v>
+        <v>0.70744976383170577</v>
       </c>
       <c r="AM133" s="6">
-        <v>1.2072263975199693</v>
+        <v>1.2072263975199555</v>
       </c>
       <c r="AN133" s="6">
-        <v>0.41543349778304306</v>
+        <v>0.41543349778302247</v>
       </c>
       <c r="AO133" s="6">
-        <v>0.77723938514852764</v>
+        <v>0.77723938514852065</v>
       </c>
       <c r="AP133" s="6">
-        <v>0.45641689779746103</v>
+        <v>0.45641689779745498</v>
       </c>
       <c r="AQ133" s="6">
-        <v>0.7311519396355497</v>
+        <v>0.73115193963553315</v>
       </c>
       <c r="AR133" s="6">
-        <v>1.8525828422760706</v>
+        <v>1.8525828422760606</v>
       </c>
       <c r="AS133" s="6">
-        <v>1.3274004566528499</v>
+        <v>1.3274004566528386</v>
       </c>
       <c r="AT133" s="6">
-        <v>0.75974028968149021</v>
+        <v>0.75974028968148533</v>
       </c>
       <c r="AU133" s="6">
-        <v>-1.6655985475714243</v>
+        <v>-1.6655985475714268</v>
       </c>
       <c r="AV133" s="6">
-        <v>0.40877765904398311</v>
+        <v>0.40877765904397412</v>
       </c>
       <c r="AW133" s="6">
-        <v>2.0481917531482776</v>
+        <v>2.0481917531482834</v>
       </c>
       <c r="AX133" s="6">
-        <v>1.0496331659505749</v>
+        <v>1.04963316595057</v>
       </c>
       <c r="AY133" s="6">
-        <v>1.9067222854653649</v>
+        <v>1.9067222854653592</v>
       </c>
       <c r="AZ133" s="6">
-        <v>2.3226676825035311</v>
+        <v>2.3226676825035293</v>
       </c>
       <c r="BA133" s="6">
-        <v>6.8648895665056191</v>
+        <v>6.8648895665056218</v>
       </c>
     </row>
     <row r="134" spans="1:53" x14ac:dyDescent="0.2">
@@ -23235,160 +23235,321 @@
         <v>43344</v>
       </c>
       <c r="B134" s="6">
-        <v>1.0522343783102608</v>
+        <v>0.7963188259252737</v>
       </c>
       <c r="C134" s="6">
-        <v>3.6720414799299905</v>
+        <v>4.1105875310201982</v>
       </c>
       <c r="D134" s="6">
-        <v>1.4629608616867955</v>
+        <v>0.75786663703326351</v>
       </c>
       <c r="E134" s="6">
-        <v>-0.3908115086472253</v>
+        <v>-7.9939298609803672E-2</v>
       </c>
       <c r="F134" s="6">
-        <v>1.4564112314512327</v>
+        <v>2.3147224657790133</v>
       </c>
       <c r="G134" s="6">
-        <v>3.09477662235747</v>
+        <v>3.0291308711857456</v>
       </c>
       <c r="H134" s="6">
-        <v>5.9840635393158443</v>
+        <v>5.6036046927912695</v>
       </c>
       <c r="I134" s="6">
-        <v>3.300181618255039</v>
+        <v>4.2566130935641056</v>
       </c>
       <c r="J134" s="6">
-        <v>-2.3361771855428177</v>
+        <v>-2.1885380808107953</v>
       </c>
       <c r="K134" s="6">
-        <v>8.3817889670375791</v>
+        <v>7.5055057439690724</v>
       </c>
       <c r="L134" s="6">
-        <v>5.3018233838402464</v>
+        <v>5.7310362201655165</v>
       </c>
       <c r="M134" s="6">
-        <v>2.5514344024046309</v>
+        <v>3.3136168693798549</v>
       </c>
       <c r="N134" s="6">
-        <v>5.9613501052124978</v>
+        <v>5.5849332309488737</v>
       </c>
       <c r="O134" s="6">
-        <v>2.9858458151552734</v>
+        <v>3.1197541963912312</v>
       </c>
       <c r="P134" s="6">
-        <v>3.9140827761526324</v>
+        <v>4.2083460006463405</v>
       </c>
       <c r="Q134" s="6">
-        <v>-1.5223060286852237</v>
+        <v>-1.3558711913236343</v>
       </c>
       <c r="R134" s="6">
-        <v>3.3747213488328978</v>
+        <v>3.962772084193499</v>
       </c>
       <c r="S134" s="6">
-        <v>3.9619917871775434</v>
+        <v>3.8773721317097762</v>
       </c>
       <c r="T134" s="6">
-        <v>0.15406220263516718</v>
+        <v>0.33500901781609149</v>
       </c>
       <c r="U134" s="6">
-        <v>3.9102256034066385</v>
+        <v>3.4316523133506487</v>
       </c>
       <c r="V134" s="6">
-        <v>0.45678848329375038</v>
+        <v>0.62425109748660024</v>
       </c>
       <c r="W134" s="6">
-        <v>5.2589557875999754E-2</v>
+        <v>0.40657925572568615</v>
       </c>
       <c r="X134" s="6">
-        <v>1.9798699200510608</v>
+        <v>2.3145840609126007</v>
       </c>
       <c r="Y134" s="6">
-        <v>3.4438878365763426</v>
+        <v>3.4438878365763439</v>
       </c>
       <c r="Z134" s="6">
-        <v>1.7937004490976503</v>
+        <v>1.3944111101261818</v>
       </c>
       <c r="AA134" s="6">
-        <v>-3.5843990368646348</v>
+        <v>-3.0744281972678191</v>
       </c>
       <c r="AB134" s="6">
-        <v>3.8437224374123682</v>
+        <v>3.8437224374123788</v>
       </c>
       <c r="AC134" s="6">
-        <v>5.3115746374478068</v>
+        <v>5.6180953441553969</v>
       </c>
       <c r="AD134" s="6">
-        <v>1.4217114184639936</v>
+        <v>1.5018093985164529</v>
       </c>
       <c r="AE134" s="6">
-        <v>3.6050629949211426</v>
+        <v>3.3948900675429328</v>
       </c>
       <c r="AF134" s="6">
-        <v>-1.175932182923729</v>
+        <v>-1.4325389957574342</v>
       </c>
       <c r="AG134" s="6">
-        <v>1.588581659457343</v>
+        <v>1.3632559595106359</v>
       </c>
       <c r="AH134" s="6">
-        <v>3.7229359134889268</v>
+        <v>3.6064994899671401</v>
       </c>
       <c r="AI134" s="6">
-        <v>2.338518077886631</v>
+        <v>2.7094262082451226</v>
       </c>
       <c r="AJ134" s="6">
-        <v>1.4336733397987642</v>
+        <v>1.7734257684028656</v>
       </c>
       <c r="AK134" s="6">
-        <v>4.2781644656229068</v>
+        <v>4.4703460722482165</v>
       </c>
       <c r="AL134" s="6">
-        <v>1.871878383857442</v>
+        <v>2.3987005184063293</v>
       </c>
       <c r="AM134" s="6">
-        <v>3.4545892509059302</v>
+        <v>3.8426562485012425</v>
       </c>
       <c r="AN134" s="6">
-        <v>2.8695880409378649</v>
+        <v>2.9316651854145679</v>
       </c>
       <c r="AO134" s="6">
-        <v>2.3225540541382172</v>
+        <v>2.4023581675149774</v>
       </c>
       <c r="AP134" s="6">
-        <v>0.85522522948878532</v>
+        <v>-0.21921124954046942</v>
       </c>
       <c r="AQ134" s="6">
-        <v>2.1133861352129091</v>
+        <v>2.6283250715927808</v>
       </c>
       <c r="AR134" s="6">
-        <v>4.8159858236230635</v>
+        <v>4.5569720909407616</v>
       </c>
       <c r="AS134" s="6">
-        <v>3.9105833036215003</v>
+        <v>4.0857832192682091</v>
       </c>
       <c r="AT134" s="6">
-        <v>5.3244025572225309E-2</v>
+        <v>1.2898487838363222</v>
       </c>
       <c r="AU134" s="6">
-        <v>0.88975471677911222</v>
+        <v>2.3976911778911338</v>
       </c>
       <c r="AV134" s="6">
-        <v>1.5363781357180926</v>
+        <v>1.7355915736708551</v>
       </c>
       <c r="AW134" s="6">
-        <v>3.074710583502541</v>
+        <v>3.7297505954911707</v>
       </c>
       <c r="AX134" s="6">
-        <v>5.5445570230942076</v>
+        <v>6.0651771894453859</v>
       </c>
       <c r="AY134" s="6">
-        <v>2.2926049271702134</v>
+        <v>2.6030056026298398</v>
       </c>
       <c r="AZ134" s="6">
-        <v>2.4785731592905584</v>
+        <v>2.7937809013985726</v>
       </c>
       <c r="BA134" s="6">
-        <v>8.3585884764827973</v>
+        <v>9.8583776982897682</v>
+      </c>
+    </row>
+    <row r="135" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A135" s="5">
+        <v>43374</v>
+      </c>
+      <c r="B135" s="6">
+        <v>0.89028384106915603</v>
+      </c>
+      <c r="C135" s="6">
+        <v>-0.20838298732660993</v>
+      </c>
+      <c r="D135" s="6">
+        <v>-2.3524774276216123</v>
+      </c>
+      <c r="E135" s="6">
+        <v>-4.4003249305351408</v>
+      </c>
+      <c r="F135" s="6">
+        <v>-0.25213866774239246</v>
+      </c>
+      <c r="G135" s="6">
+        <v>-2.5638336570555071</v>
+      </c>
+      <c r="H135" s="6">
+        <v>0.46729415175027905</v>
+      </c>
+      <c r="I135" s="6">
+        <v>0.82354331470505771</v>
+      </c>
+      <c r="J135" s="6">
+        <v>-3.8129288192124173</v>
+      </c>
+      <c r="K135" s="6">
+        <v>-2.6011063861862196</v>
+      </c>
+      <c r="L135" s="6">
+        <v>-0.32118864060402791</v>
+      </c>
+      <c r="M135" s="6">
+        <v>-1.8559385270674202</v>
+      </c>
+      <c r="N135" s="6">
+        <v>-2.7407087011661599</v>
+      </c>
+      <c r="O135" s="6">
+        <v>-1.9104585328419299</v>
+      </c>
+      <c r="P135" s="6">
+        <v>-7.9669689985093162E-2</v>
+      </c>
+      <c r="Q135" s="6">
+        <v>-2.6584907328583802</v>
+      </c>
+      <c r="R135" s="6">
+        <v>0.97035133742211443</v>
+      </c>
+      <c r="S135" s="6">
+        <v>-0.47498133163317752</v>
+      </c>
+      <c r="T135" s="6">
+        <v>-0.66094229167942797</v>
+      </c>
+      <c r="U135" s="6">
+        <v>1.1382098085228431</v>
+      </c>
+      <c r="V135" s="6">
+        <v>0.49770311455368654</v>
+      </c>
+      <c r="W135" s="6">
+        <v>-8.1938247922405569</v>
+      </c>
+      <c r="X135" s="6">
+        <v>-0.70827873508557104</v>
+      </c>
+      <c r="Y135" s="6">
+        <v>-0.1107790672203957</v>
+      </c>
+      <c r="Z135" s="6">
+        <v>-3.1631090623454741</v>
+      </c>
+      <c r="AA135" s="6">
+        <v>-4.1819321146921382</v>
+      </c>
+      <c r="AB135" s="6">
+        <v>8.0236476364622958E-2</v>
+      </c>
+      <c r="AC135" s="6">
+        <v>-0.37368575285386585</v>
+      </c>
+      <c r="AD135" s="6">
+        <v>-4.0434092042939715</v>
+      </c>
+      <c r="AE135" s="6">
+        <v>-0.56728177877769415</v>
+      </c>
+      <c r="AF135" s="6">
+        <v>-2.4135631487049789</v>
+      </c>
+      <c r="AG135" s="6">
+        <v>-2.4690254218325736</v>
+      </c>
+      <c r="AH135" s="6">
+        <v>-0.58557129258653973</v>
+      </c>
+      <c r="AI135" s="6">
+        <v>-1.2798917142572384</v>
+      </c>
+      <c r="AJ135" s="6">
+        <v>-0.41367445903778244</v>
+      </c>
+      <c r="AK135" s="6">
+        <v>-1.3247121758297646</v>
+      </c>
+      <c r="AL135" s="6">
+        <v>7.8692570836398579E-2</v>
+      </c>
+      <c r="AM135" s="6">
+        <v>0.1437969794037976</v>
+      </c>
+      <c r="AN135" s="6">
+        <v>-3.2461473057423778</v>
+      </c>
+      <c r="AO135" s="6">
+        <v>0.45644560593786815</v>
+      </c>
+      <c r="AP135" s="6">
+        <v>-1.1984077235088599</v>
+      </c>
+      <c r="AQ135" s="6">
+        <v>0.29040882214800029</v>
+      </c>
+      <c r="AR135" s="6">
+        <v>-1.1873960803168371</v>
+      </c>
+      <c r="AS135" s="6">
+        <v>1.2814435413854348</v>
+      </c>
+      <c r="AT135" s="6">
+        <v>-2.4003085721641049</v>
+      </c>
+      <c r="AU135" s="6">
+        <v>-4.7402621415333117</v>
+      </c>
+      <c r="AV135" s="6">
+        <v>-0.75230153209548034</v>
+      </c>
+      <c r="AW135" s="6">
+        <v>-0.77222551562772557</v>
+      </c>
+      <c r="AX135" s="6">
+        <v>-1.3670646255692225</v>
+      </c>
+      <c r="AY135" s="6">
+        <v>0.60637894512224433</v>
+      </c>
+      <c r="AZ135" s="6">
+        <v>-1.3632198010097709</v>
+      </c>
+      <c r="BA135" s="6">
+        <v>3.6734486800104533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>